<commit_message>
Output updated to latest data
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 29 November 2022</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 December 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -38,69 +38,54 @@
     <t xml:space="preserve">Week</t>
   </si>
   <si>
-    <t xml:space="preserve">28 Nov 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil Justice statistics quarterly: July to September 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 December 2022</t>
+    <t xml:space="preserve">12 Dec 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Court statistics quarterly: July to September 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 December 2022</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">05 Dec 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 December 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Dec 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Court statistics quarterly: July to September 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 December 2022</t>
+    <t xml:space="preserve">Legal aid statistics: July to September 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMPPS COVID-19 statistics : November 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 December 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Dec 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 Dec 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Jan 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Jan 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Jan 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Criminal court statistics quarterly: July to September 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal aid statistics: July to September 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMPPS COVID-19 statistics : November 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 December 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Dec 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 Dec 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02 Jan 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Jan 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Jan 2023</t>
+    <t xml:space="preserve">19 January 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
   </si>
   <si>
     <t xml:space="preserve">Electronic Monitoring Statistics Publication, December 2022 </t>
   </si>
   <si>
-    <t xml:space="preserve">19 January 2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">23 Jan 2023</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">26 January 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
   </si>
   <si>
     <t xml:space="preserve">Proven reoffending statistics: January to March 2021</t>
@@ -823,35 +805,35 @@
         <v>11</v>
       </c>
       <c r="E5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -864,126 +846,126 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>51</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>4</v>
@@ -991,16 +973,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>4</v>
@@ -1008,16 +990,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>4</v>
@@ -1025,78 +1007,78 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>7</v>
@@ -1104,36 +1086,36 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -1147,80 +1129,80 @@
         <v>48</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13</v>
@@ -1228,89 +1210,89 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>17</v>
@@ -1318,16 +1300,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>17</v>
@@ -1335,16 +1317,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>17</v>
@@ -1352,78 +1334,78 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C43" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>20</v>
@@ -1431,16 +1413,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>20</v>
@@ -1448,16 +1430,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>20</v>
@@ -1465,117 +1447,117 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>26</v>
@@ -1583,113 +1565,79 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="5" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="5" t="n">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:E61">
+  <conditionalFormatting sqref="A5:E59">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1700,7 +1648,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A61">
+  <conditionalFormatting sqref="A5:A59">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changed the way the file is saved. Now it is saved in S3, and run automatically every Thursday with Airflow, and then a script downloads it from S3.
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -12,12 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 June 2023</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics
+                                            that have been pre-announced on the gov.uk release calendar as at 22 June 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -38,6 +39,9 @@
     <t xml:space="preserve">Week</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">26 Jun 2023</t>
   </si>
   <si>
@@ -48,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
   </si>
   <si>
     <t xml:space="preserve">Legal aid statistics quarterly: January to March 2023</t>
@@ -338,7 +345,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="6">
     <font>
@@ -760,18 +767,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="96.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="24.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="12.71" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -805,61 +813,73 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
         <v>26</v>
       </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
         <v>26</v>
       </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
         <v>26</v>
       </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -867,197 +887,231 @@
       <c r="E8" t="n">
         <v>27</v>
       </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>28</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>29</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>29</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>30</v>
       </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1065,78 +1119,91 @@
       <c r="E20" s="5" t="n">
         <v>31</v>
       </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>32</v>
       </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>33</v>
       </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>33</v>
       </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>33</v>
       </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1144,10 +1211,11 @@
       <c r="E25" s="5" t="n">
         <v>34</v>
       </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1155,44 +1223,51 @@
       <c r="E26" s="5" t="n">
         <v>35</v>
       </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>36</v>
       </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>37</v>
       </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1200,78 +1275,91 @@
       <c r="E29" s="5" t="n">
         <v>38</v>
       </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>39</v>
       </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>39</v>
       </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>39</v>
       </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>39</v>
       </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1279,146 +1367,171 @@
       <c r="E34" s="5" t="n">
         <v>40</v>
       </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>41</v>
       </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>42</v>
       </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>43</v>
       </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1426,180 +1539,211 @@
       <c r="E43" s="5" t="n">
         <v>44</v>
       </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>45</v>
       </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>46</v>
       </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>46</v>
       </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>46</v>
       </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>47</v>
       </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>47</v>
       </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>48</v>
       </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>49</v>
       </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>50</v>
       </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>51</v>
       </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -1607,10 +1751,11 @@
       <c r="E54" s="5" t="n">
         <v>52</v>
       </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1618,10 +1763,11 @@
       <c r="E55" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1629,10 +1775,11 @@
       <c r="E56" s="5" t="n">
         <v>2</v>
       </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -1640,77 +1787,90 @@
       <c r="E57" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="D60" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:E61">
+  <conditionalFormatting sqref="A5:F61">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Edited code to correct week dates (2024 started on a Monday and weeks were counted as starting Sunday so the first week of 2024 was being counted as the last week of 2023).
Minor formatting changes.
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -12,13 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics
-                                            that have been pre-announced on the gov.uk release calendar as at 12 October 2023</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 24 January 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -42,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">16 Oct 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 October 2023</t>
+    <t xml:space="preserve">22 Jan 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: July to September 2023 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 January 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -57,184 +56,61 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">23 Oct 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: October to December 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 October 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serious Further Offence 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender Management Statistics quarterly: April to June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Population Projections: 2023 to 2028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2022/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-agency public protection arrangements (MAPPA) annual: 2022 to 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 Oct 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 Nov 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and Landlord Possession statistics: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 November 2023</t>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: January to March 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethnicity and the Criminal Justice System 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Justice Statistics: 2022 to 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: January 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Jan 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 February 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 February 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 February 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">13 Nov 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal Justice System statistics quarterly: June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 November 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: April to June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 Nov 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2022 to 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 November 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethnicity and the Criminal Justice System 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 Nov 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2022 to 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 November 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04 Dec 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 Dec 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Dec 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Dec 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication , December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 January 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: July to September 2023 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 January 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: January to March 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitoring Statistics Quarterly Publication, March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: January 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 February 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 February 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2023</t>
+    <t xml:space="preserve">ad-hoc</t>
   </si>
   <si>
     <t xml:space="preserve">26 Feb 2024</t>
@@ -243,33 +119,42 @@
     <t xml:space="preserve">04 Mar 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">11 Mar 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">18 Mar 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 March 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">25 Mar 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">01 Apr 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">08 Apr 2024</t>
   </si>
   <si>
@@ -279,67 +164,103 @@
     <t xml:space="preserve">22 Apr 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 April 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: April 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: April to June 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">29 Apr 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: April to June 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">06 May 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Coroners statistics 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 May 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">13 May 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: February to April 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">20 May 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">27 May 2024</t>
   </si>
   <si>
     <t xml:space="preserve">03 Jun 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 Jun 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">17 Jun 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 Jun 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 June 2024</t>
+    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: January to March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">01 Jul 2024</t>
@@ -348,34 +269,235 @@
     <t xml:space="preserve">08 Jul 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 July 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">15 Jul 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 July 2024</t>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">22 Jul 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: July 2022 to September 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMPPS Annual Digest, April 2023 to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">29 Jul 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Proven reoffending statistics: July 2022 to September 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMPPS Annual Digest, April 2022 to March 2024</t>
+    <t xml:space="preserve">05 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June with 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 August 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 August 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: April to June 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 January 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="6">
     <font>
@@ -797,19 +919,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="108.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="18.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -861,7 +983,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -869,19 +991,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -889,19 +1011,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -909,19 +1031,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -929,19 +1051,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -949,19 +1071,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -969,19 +1091,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -989,39 +1111,31 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1031,29 +1145,37 @@
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1061,59 +1183,51 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1121,19 +1235,19 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1141,19 +1255,19 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1161,23 +1275,15 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E21" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
@@ -1190,10 +1296,10 @@
         <v>43</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1201,19 +1307,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1221,19 +1327,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1241,95 +1347,95 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1337,19 +1443,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1357,19 +1463,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1377,19 +1483,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1397,39 +1503,31 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1437,19 +1535,19 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1457,31 +1555,39 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1489,19 +1595,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1509,19 +1615,19 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1529,55 +1635,63 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1585,31 +1699,39 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1617,19 +1739,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1637,55 +1759,71 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="B50" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1693,19 +1831,19 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1713,19 +1851,19 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1733,19 +1871,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1753,19 +1891,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1773,43 +1911,59 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
@@ -1817,39 +1971,31 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>13</v>
@@ -1857,111 +2003,119 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>13</v>
@@ -1969,31 +2123,39 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="D70" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>13</v>
@@ -2001,26 +2163,510 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E81" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5" t="n">
+        <v>52</v>
+      </c>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E100" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F71">
+  <conditionalFormatting sqref="A5:F100">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2031,7 +2677,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A71">
+  <conditionalFormatting sqref="A5:A100">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed week commencing dates issue and added renv lines.
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 24 January 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 February 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,60 +41,36 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">22 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: July to September 2023 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 January 2024</t>
+    <t xml:space="preserve">29 Jan 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Population Projections: 2023 to 2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 February 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 February 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: January to March 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethnicity and the Criminal Justice System 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youth Justice Statistics: 2022 to 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: January 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Jan 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 February 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 February 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2023</t>
   </si>
   <si>
@@ -107,9 +83,6 @@
     <t xml:space="preserve">22 February 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
     <t xml:space="preserve">ad-hoc</t>
   </si>
   <si>
@@ -464,6 +437,9 @@
     <t xml:space="preserve">23 Dec 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">29 Dec 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">06 Jan 2025</t>
   </si>
   <si>
@@ -474,9 +450,6 @@
   </si>
   <si>
     <t xml:space="preserve">27 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03 Feb 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
@@ -497,7 +470,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="6">
     <font>
@@ -508,14 +481,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <b/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <b/>
     </font>
@@ -563,8 +536,8 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -919,10 +892,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -935,7 +908,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -950,22 +923,22 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -983,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -991,39 +964,31 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -1031,19 +996,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1051,59 +1016,51 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1111,31 +1068,39 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1143,39 +1108,31 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1183,123 +1140,115 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1307,19 +1256,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1327,19 +1276,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1347,27 +1296,43 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
@@ -1377,7 +1342,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -1392,10 +1357,10 @@
         <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1403,19 +1368,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1423,19 +1388,19 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1443,19 +1408,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1463,19 +1428,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1483,19 +1448,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1503,35 +1468,27 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
@@ -1547,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1555,19 +1512,19 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1575,19 +1532,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1595,19 +1552,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1615,19 +1572,19 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1635,43 +1592,51 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1679,19 +1644,19 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1699,19 +1664,19 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1719,19 +1684,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1739,19 +1704,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1759,31 +1724,39 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1791,19 +1764,19 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1811,19 +1784,19 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1833,37 +1806,29 @@
       <c r="A52" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="E52" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="D53" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1871,19 +1836,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1891,19 +1856,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1911,95 +1876,63 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C60" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
@@ -2015,7 +1948,7 @@
         <v>12</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -2032,10 +1965,10 @@
         <v>106</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -2043,27 +1976,43 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
@@ -2073,7 +2022,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F65" s="5"/>
     </row>
@@ -2085,7 +2034,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -2093,49 +2042,49 @@
       <c r="A67" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="B67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>13</v>
@@ -2143,19 +2092,19 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>13</v>
@@ -2163,19 +2112,19 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="D71" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>13</v>
@@ -2183,43 +2132,59 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E72" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>13</v>
@@ -2233,7 +2198,7 @@
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F75" s="5"/>
     </row>
@@ -2241,37 +2206,29 @@
       <c r="A76" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B77" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="D77" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E77" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>13</v>
@@ -2279,19 +2236,19 @@
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>129</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E78" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>13</v>
@@ -2299,19 +2256,19 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E79" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>13</v>
@@ -2319,19 +2276,19 @@
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>13</v>
@@ -2339,63 +2296,63 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E83" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F83" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E84" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>13</v>
@@ -2403,63 +2360,39 @@
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C86" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B87" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
@@ -2469,7 +2402,7 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -2481,7 +2414,7 @@
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F89" s="5"/>
     </row>
@@ -2496,10 +2429,10 @@
         <v>147</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E90" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>13</v>
@@ -2516,10 +2449,10 @@
         <v>147</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E91" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>13</v>
@@ -2527,146 +2460,46 @@
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E92" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F92" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B93" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
+      <c r="C93" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E93" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E97" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F97" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E98" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E99" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E100" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F100" s="5" t="s">
+      <c r="F93" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F100">
+  <conditionalFormatting sqref="A5:F93">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2677,7 +2510,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A100">
+  <conditionalFormatting sqref="A5:A93">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
dates without a given day have been updated to last day of the month
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 February 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 16 February 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,28 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">29 Jan 2024</t>
+    <t xml:space="preserve">19 Feb 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 February 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad-hoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 Feb 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Prison Population Projections: 2023 to 2028</t>
   </si>
   <si>
-    <t xml:space="preserve">1 February 2024</t>
+    <t xml:space="preserve">29 February 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
@@ -56,39 +71,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">05 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 February 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 February 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 Feb 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">04 Mar 2024</t>
   </si>
   <si>
@@ -117,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve">28 March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug and alcohol treatment for victims and suspects of homicide in England</t>
   </si>
   <si>
     <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
@@ -481,14 +466,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <b/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <b/>
     </font>
@@ -536,8 +521,8 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -908,7 +893,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -923,22 +908,22 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -956,7 +941,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -966,589 +951,597 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6"/>
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
@@ -1561,457 +1554,449 @@
         <v>72</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D43" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C45" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C63" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65">
@@ -2022,7 +2007,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F65" s="5"/>
     </row>
@@ -2030,281 +2015,289 @@
       <c r="A66" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="B66" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E66" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D67" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C69" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E71" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B74" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="D74" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="B76" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="D77" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E77" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B78" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B80" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="D80" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E81" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F81" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
@@ -2314,7 +2307,7 @@
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F82" s="5"/>
     </row>
@@ -2322,184 +2315,132 @@
       <c r="A83" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="D87" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E87" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F87" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E88" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F88" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E89" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F89" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>146</v>
-      </c>
       <c r="C90" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E90" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E93" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F93">
+  <conditionalFormatting sqref="A5:F90">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2510,7 +2451,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A93">
+  <conditionalFormatting sqref="A5:A90">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated forward look 08.03.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 29 February 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,49 +41,37 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">26 Feb 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Population Projections: 2023 to 2028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 February 2024</t>
+    <t xml:space="preserve">11 Mar 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Intensive Intervention and Risk Management Services (IIRMS) Publication, March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 March 2024</t>
+    <t xml:space="preserve">ad-hoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Mar 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
   </si>
   <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Mar 2024</t>
+    <t xml:space="preserve">21 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">25 Mar 2024</t>
@@ -932,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -940,62 +928,62 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="n">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -1009,10 +997,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1020,28 +1008,36 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>13</v>
@@ -1052,92 +1048,92 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E16" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
@@ -1148,16 +1144,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>17</v>
@@ -1168,16 +1164,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>17</v>
@@ -1188,16 +1184,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>17</v>
@@ -1208,39 +1204,31 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="E21" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1250,29 +1238,37 @@
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1280,16 +1276,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>20</v>
@@ -1300,16 +1296,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>20</v>
@@ -1320,13 +1316,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>12</v>
@@ -1340,83 +1336,83 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1424,19 +1420,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1444,19 +1440,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1466,37 +1462,29 @@
       <c r="A35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D36" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1506,29 +1494,37 @@
       <c r="A37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1545,10 +1541,10 @@
         <v>72</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1565,10 +1561,10 @@
         <v>72</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1576,16 +1572,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C41" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>30</v>
@@ -1596,16 +1592,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>30</v>
@@ -1616,16 +1612,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>30</v>
@@ -1636,16 +1632,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>30</v>
@@ -1656,16 +1652,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>30</v>
@@ -1676,39 +1672,31 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1718,29 +1706,37 @@
       <c r="A48" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1750,114 +1746,114 @@
       <c r="A50" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>39</v>
@@ -1868,16 +1864,16 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>39</v>
@@ -1888,55 +1884,47 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
@@ -1946,7 +1934,7 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -1961,10 +1949,10 @@
         <v>106</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1972,28 +1960,36 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="C65" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>44</v>
@@ -2004,16 +2000,16 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>44</v>
@@ -2024,16 +2020,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>44</v>
@@ -2044,16 +2040,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>44</v>
@@ -2064,67 +2060,67 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E72" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
@@ -2137,10 +2133,10 @@
         <v>120</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>13</v>
@@ -2160,7 +2156,7 @@
         <v>12</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>13</v>
@@ -2170,178 +2166,178 @@
       <c r="A75" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E78" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F78" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="D84" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E84" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E85" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F85" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="C86" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E86" s="5" t="n">
         <v>5</v>
@@ -2352,16 +2348,16 @@
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E87" s="5" t="n">
         <v>5</v>
@@ -2370,48 +2366,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E88" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E89" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F89">
+  <conditionalFormatting sqref="A5:F87">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2422,7 +2378,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A89">
+  <conditionalFormatting sqref="A5:A87">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look update 15.03.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 March 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 15 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -44,43 +44,40 @@
     <t xml:space="preserve">11 Mar 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 March 2024</t>
+    <t xml:space="preserve">Ad-Hoc Intensive Intervention and Risk Management Services (IIRMS) Publication, March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad-hoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Mar 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
+    <t xml:space="preserve">25 Mar 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Intensive Intervention and Risk Management Services (IIRMS) Publication, March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
@@ -928,1446 +925,1406 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="E11" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+        <v>123</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="B76" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E82" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F82" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="B83" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E83" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F83" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B84" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="D84" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E84" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E85" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E87" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F87">
+  <conditionalFormatting sqref="A5:F85">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2378,7 +2335,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A87">
+  <conditionalFormatting sqref="A5:A85">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
update forward look 22.03.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 15 March 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 22 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,82 +41,61 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">11 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Intensive Intervention and Risk Management Services (IIRMS) Publication, March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 March 2024</t>
+    <t xml:space="preserve">25 Mar 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Female Offender Metrics Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 March 2024</t>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 April 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: April 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: April to June 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: April to June 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
   </si>
   <si>
     <t xml:space="preserve">29 Apr 2024</t>
@@ -917,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -925,19 +904,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -945,13 +924,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -960,94 +939,94 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1056,18 +1035,18 @@
         <v>17</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1076,18 +1055,18 @@
         <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1096,110 +1075,110 @@
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>12</v>
@@ -1208,1123 +1187,1083 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F24" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>30</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="C64" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C66" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="C70" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E74" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F74" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E80" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F80" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E81" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F81" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E82" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E83" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E84" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F85">
+  <conditionalFormatting sqref="A5:F83">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2335,7 +2274,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A85">
+  <conditionalFormatting sqref="A5:A83">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look stats update 28.03.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 22 March 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">25 Mar 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 March 2024</t>
+    <t xml:space="preserve">22 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 April 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,30 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 April 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
   </si>
   <si>
@@ -95,37 +71,37 @@
     <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
   </si>
   <si>
+    <t xml:space="preserve">29 Apr 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroners statistics 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: February to April 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: December 2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroners statistics 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: February to April 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: December 2023</t>
   </si>
   <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2024</t>
@@ -896,7 +872,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -916,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -936,7 +912,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -944,75 +920,91 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" t="n">
-        <v>14</v>
-      </c>
-      <c r="F8"/>
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1020,19 +1012,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1040,19 +1032,19 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1060,19 +1052,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1080,19 +1072,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1100,71 +1092,63 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1172,19 +1156,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1192,19 +1176,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1212,19 +1196,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1232,43 +1216,51 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1276,19 +1268,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1296,19 +1288,19 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1316,19 +1308,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1336,19 +1328,19 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1358,29 +1350,37 @@
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1388,19 +1388,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1408,19 +1408,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1428,16 +1428,16 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>30</v>
@@ -1448,39 +1448,31 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1488,19 +1480,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1508,19 +1500,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1528,111 +1520,79 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1640,39 +1600,63 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
@@ -1682,7 +1666,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1694,7 +1678,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1709,10 +1693,10 @@
         <v>86</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1720,39 +1704,31 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1760,19 +1736,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1780,43 +1756,59 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1824,71 +1816,63 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="D61" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -1896,19 +1880,19 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1916,19 +1900,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1936,19 +1920,19 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1956,43 +1940,43 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -2000,19 +1984,19 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>13</v>
@@ -2020,43 +2004,27 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C69" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
@@ -2066,7 +2034,7 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="F71" s="5"/>
     </row>
@@ -2078,7 +2046,7 @@
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="F72" s="5"/>
     </row>
@@ -2086,37 +2054,29 @@
       <c r="A73" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="D74" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E74" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>13</v>
@@ -2124,146 +2084,66 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F78" s="5"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E80" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F80" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E81" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E83" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F83" s="5" t="s">
+      <c r="F77" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F83">
+  <conditionalFormatting sqref="A5:F77">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2274,7 +2154,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A83">
+  <conditionalFormatting sqref="A5:A77">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
update to stats forward look 05.04.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 March 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 05 April 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -101,27 +101,27 @@
     <t xml:space="preserve">Criminal justice statistics quarterly: December 2023</t>
   </si>
   <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Jun 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil justice statistics: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 June 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 Jun 2024</t>
   </si>
   <si>
@@ -381,6 +381,21 @@
   </si>
   <si>
     <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 February 2025</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1096,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>20</v>
@@ -1095,13 +1110,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>20</v>
@@ -1112,7 +1127,7 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1124,7 +1139,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1136,16 +1151,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>23</v>
@@ -1165,7 +1180,7 @@
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>24</v>
@@ -1185,7 +1200,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>25</v>
@@ -1205,7 +1220,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>26</v>
@@ -1225,7 +1240,7 @@
         <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>26</v>
@@ -1257,7 +1272,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>28</v>
@@ -1277,7 +1292,7 @@
         <v>52</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>29</v>
@@ -1297,7 +1312,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>29</v>
@@ -1317,7 +1332,7 @@
         <v>56</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>30</v>
@@ -1337,7 +1352,7 @@
         <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>30</v>
@@ -1357,7 +1372,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>30</v>
@@ -1377,7 +1392,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>30</v>
@@ -1397,7 +1412,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>30</v>
@@ -1417,7 +1432,7 @@
         <v>56</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>30</v>
@@ -1437,7 +1452,7 @@
         <v>56</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>30</v>
@@ -1469,7 +1484,7 @@
         <v>66</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>32</v>
@@ -1509,7 +1524,7 @@
         <v>69</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>33</v>
@@ -1589,7 +1604,7 @@
         <v>78</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>39</v>
@@ -1609,7 +1624,7 @@
         <v>78</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>39</v>
@@ -1629,7 +1644,7 @@
         <v>78</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>39</v>
@@ -1649,7 +1664,7 @@
         <v>78</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>39</v>
@@ -1693,7 +1708,7 @@
         <v>86</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>42</v>
@@ -1725,7 +1740,7 @@
         <v>90</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>44</v>
@@ -1745,7 +1760,7 @@
         <v>90</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>44</v>
@@ -1765,7 +1780,7 @@
         <v>90</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>44</v>
@@ -1785,7 +1800,7 @@
         <v>90</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>44</v>
@@ -1805,7 +1820,7 @@
         <v>90</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>44</v>
@@ -1825,7 +1840,7 @@
         <v>90</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>44</v>
@@ -1869,7 +1884,7 @@
         <v>100</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>47</v>
@@ -1909,7 +1924,7 @@
         <v>104</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>48</v>
@@ -1929,7 +1944,7 @@
         <v>104</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>48</v>
@@ -1973,7 +1988,7 @@
         <v>110</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>51</v>
@@ -1993,7 +2008,7 @@
         <v>110</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>51</v>
@@ -2073,7 +2088,7 @@
         <v>119</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E74" s="5" t="n">
         <v>5</v>
@@ -2093,7 +2108,7 @@
         <v>119</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>5</v>
@@ -2113,7 +2128,7 @@
         <v>119</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E76" s="5" t="n">
         <v>5</v>
@@ -2133,7 +2148,7 @@
         <v>119</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E77" s="5" t="n">
         <v>5</v>
@@ -2142,8 +2157,52 @@
         <v>13</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F77">
+  <conditionalFormatting sqref="A5:F80">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2154,7 +2213,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A77">
+  <conditionalFormatting sqref="A5:A80">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
update to script and forward look weekly update 12.04.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 05 April 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 April 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -347,6 +347,9 @@
     <t xml:space="preserve">19 December 2024</t>
   </si>
   <si>
+    <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Criminal court statistics quarterly: July to September 2024</t>
   </si>
   <si>
@@ -374,6 +377,9 @@
     <t xml:space="preserve">30 January 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
   </si>
   <si>
@@ -396,6 +402,48 @@
   </si>
   <si>
     <t xml:space="preserve">20 February 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 April 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: October to December 2024</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1460,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>30</v>
@@ -2019,15 +2067,23 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
@@ -2037,7 +2093,7 @@
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="F70" s="5"/>
     </row>
@@ -2049,7 +2105,7 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" s="5"/>
     </row>
@@ -2061,7 +2117,7 @@
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" s="5"/>
     </row>
@@ -2073,7 +2129,7 @@
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" s="5"/>
     </row>
@@ -2081,31 +2137,23 @@
       <c r="A74" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B75" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>35</v>
@@ -2119,13 +2167,13 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>35</v>
@@ -2139,13 +2187,13 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>35</v>
@@ -2159,50 +2207,234 @@
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+      <c r="C78" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E78" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F78" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E79" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F79" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E80" s="5" t="n">
+      <c r="B82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E82" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F82" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="F92" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F80">
+  <conditionalFormatting sqref="A5:F92">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2213,7 +2445,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A80">
+  <conditionalFormatting sqref="A5:A92">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
update stats forward look 26.04.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 18 April 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 26 April 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">22 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 April 2024</t>
+    <t xml:space="preserve">06 May 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroners statistics 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 May 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,33 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Offender management statistics quarterly: October to December 2023  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: April to June 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Apr 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 May 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroners statistics 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 May 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">13 May 2024</t>
   </si>
   <si>
@@ -95,6 +68,12 @@
     <t xml:space="preserve">Mortgage and landlord possession statistics: February to April 2023</t>
   </si>
   <si>
+    <t xml:space="preserve">Unpaid Work Management Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
     <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2023</t>
   </si>
   <si>
@@ -119,9 +98,6 @@
     <t xml:space="preserve">6 June 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 Jun 2024</t>
   </si>
   <si>
@@ -443,7 +419,58 @@
     <t xml:space="preserve">24 April 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Offender management statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Jul 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Jul 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Jul 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Jul 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 July 2025</t>
   </si>
 </sst>
 </file>
@@ -935,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -943,19 +970,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -963,19 +990,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -983,19 +1010,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1003,19 +1030,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1023,19 +1050,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -1043,71 +1070,63 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1115,19 +1134,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1135,19 +1154,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5" t="n">
         <v>25</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1155,19 +1174,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1175,43 +1194,51 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1219,19 +1246,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1239,19 +1266,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1259,19 +1286,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1279,19 +1306,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1301,29 +1328,37 @@
       <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1331,19 +1366,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1351,19 +1386,19 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1371,13 +1406,13 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>12</v>
@@ -1391,39 +1426,31 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1431,19 +1458,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1451,19 +1478,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1471,111 +1498,79 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1583,39 +1578,63 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
@@ -1625,7 +1644,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1637,7 +1656,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1652,10 +1671,10 @@
         <v>78</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1663,39 +1682,31 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1703,19 +1714,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1723,43 +1734,59 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1767,71 +1794,63 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1839,19 +1858,19 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1859,19 +1878,19 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1879,19 +1898,19 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
@@ -1899,43 +1918,43 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -1943,19 +1962,19 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1963,19 +1982,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1983,23 +2002,15 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
@@ -2009,7 +2020,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F65" s="5"/>
     </row>
@@ -2021,7 +2032,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -2029,57 +2040,41 @@
       <c r="A67" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="D69" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>13</v>
@@ -2087,51 +2082,83 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E72" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
@@ -2141,7 +2168,7 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F74" s="5"/>
     </row>
@@ -2149,37 +2176,29 @@
       <c r="A75" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>13</v>
@@ -2187,63 +2206,39 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B77" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
@@ -2253,7 +2248,7 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F80" s="5"/>
     </row>
@@ -2261,33 +2256,33 @@
       <c r="A81" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="B81" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E81" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F81" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
@@ -2297,7 +2292,7 @@
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F83" s="5"/>
     </row>
@@ -2309,7 +2304,7 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F84" s="5"/>
     </row>
@@ -2317,41 +2312,57 @@
       <c r="A85" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="B85" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E85" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F85" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E86" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F86" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="D87" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E87" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>13</v>
@@ -2365,7 +2376,7 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -2377,7 +2388,7 @@
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F89" s="5"/>
     </row>
@@ -2389,7 +2400,7 @@
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F90" s="5"/>
     </row>
@@ -2397,44 +2408,144 @@
       <c r="A91" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
       <c r="E91" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F91" s="5"/>
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C92" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E92" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F92" s="5" t="s">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F101" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F92">
+  <conditionalFormatting sqref="A5:F101">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2445,7 +2556,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A92">
+  <conditionalFormatting sqref="A5:A101">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
update weekly forward look 03.05.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 26 April 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 03 May 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -101,10 +101,13 @@
     <t xml:space="preserve">10 Jun 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Estimates of children with a parent in prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">17 Jun 2024</t>
@@ -1154,19 +1157,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1174,19 +1177,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1194,16 +1197,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>26</v>
@@ -1214,51 +1217,51 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1266,13 +1269,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1286,19 +1289,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1306,16 +1309,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>30</v>
@@ -1326,13 +1329,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>19</v>
@@ -1346,16 +1349,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>30</v>
@@ -1366,13 +1369,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>12</v>
@@ -1386,16 +1389,16 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>30</v>
@@ -1406,16 +1409,16 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>30</v>
@@ -1426,51 +1429,51 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1478,16 +1481,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>33</v>
@@ -1498,15 +1501,23 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
@@ -1516,7 +1527,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="5"/>
     </row>
@@ -1528,7 +1539,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -1540,7 +1551,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -1552,7 +1563,7 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="5"/>
     </row>
@@ -1560,31 +1571,23 @@
       <c r="A39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>19</v>
@@ -1598,13 +1601,13 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>19</v>
@@ -1618,13 +1621,13 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>19</v>
@@ -1638,15 +1641,23 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
@@ -1656,7 +1667,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1664,63 +1675,55 @@
       <c r="A45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>19</v>
@@ -1734,13 +1737,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>19</v>
@@ -1754,13 +1757,13 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>19</v>
@@ -1774,13 +1777,13 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>19</v>
@@ -1794,13 +1797,13 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>19</v>
@@ -1814,15 +1817,23 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
@@ -1832,7 +1843,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F54" s="5"/>
     </row>
@@ -1840,34 +1851,26 @@
       <c r="A55" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>47</v>
@@ -1878,19 +1881,19 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1898,13 +1901,13 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>19</v>
@@ -1918,15 +1921,23 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
@@ -1936,7 +1947,7 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -1944,31 +1955,23 @@
       <c r="A61" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>19</v>
@@ -1982,13 +1985,13 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>19</v>
@@ -2002,15 +2005,23 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
@@ -2020,7 +2031,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="F65" s="5"/>
     </row>
@@ -2032,7 +2043,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -2044,7 +2055,7 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" s="5"/>
     </row>
@@ -2056,7 +2067,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" s="5"/>
     </row>
@@ -2064,31 +2075,23 @@
       <c r="A69" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>19</v>
@@ -2102,13 +2105,13 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>19</v>
@@ -2122,13 +2125,13 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>19</v>
@@ -2142,13 +2145,13 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>19</v>
@@ -2162,15 +2165,23 @@
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E74" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F74" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
@@ -2180,7 +2191,7 @@
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="5"/>
     </row>
@@ -2188,33 +2199,33 @@
       <c r="A76" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
@@ -2224,7 +2235,7 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" s="5"/>
     </row>
@@ -2236,7 +2247,7 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F79" s="5"/>
     </row>
@@ -2248,7 +2259,7 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F80" s="5"/>
     </row>
@@ -2256,33 +2267,33 @@
       <c r="A81" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="D82" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E82" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F82" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
@@ -2292,7 +2303,7 @@
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F83" s="5"/>
     </row>
@@ -2304,7 +2315,7 @@
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F84" s="5"/>
     </row>
@@ -2312,31 +2323,23 @@
       <c r="A85" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>19</v>
@@ -2350,13 +2353,13 @@
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>19</v>
@@ -2370,15 +2373,23 @@
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
+      <c r="C88" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E88" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F88" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
@@ -2388,7 +2399,7 @@
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F89" s="5"/>
     </row>
@@ -2400,7 +2411,7 @@
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F90" s="5"/>
     </row>
@@ -2412,7 +2423,7 @@
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F91" s="5"/>
     </row>
@@ -2424,7 +2435,7 @@
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F92" s="5"/>
     </row>
@@ -2436,7 +2447,7 @@
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F93" s="5"/>
     </row>
@@ -2448,7 +2459,7 @@
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F94" s="5"/>
     </row>
@@ -2460,7 +2471,7 @@
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F95" s="5"/>
     </row>
@@ -2472,7 +2483,7 @@
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F96" s="5"/>
     </row>
@@ -2484,7 +2495,7 @@
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F97" s="5"/>
     </row>
@@ -2496,7 +2507,7 @@
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F98" s="5"/>
     </row>
@@ -2508,7 +2519,7 @@
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F99" s="5"/>
     </row>
@@ -2520,7 +2531,7 @@
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F100" s="5"/>
     </row>
@@ -2528,24 +2539,36 @@
       <c r="A101" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="B102" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E101" s="5" t="n">
+      <c r="C102" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E102" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F102" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F101">
+  <conditionalFormatting sqref="A5:F102">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2556,7 +2579,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A101">
+  <conditionalFormatting sqref="A5:A102">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 31.05.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 23 May 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 31 May 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -59,66 +59,60 @@
     <t xml:space="preserve">10 Jun 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Offender Employment Outcomes Ad Hoc</t>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">13 June 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">ad-hoc</t>
+    <t xml:space="preserve">17 Jun 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Jun 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Estimates of children with a parent in prison</t>
   </si>
   <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">22 Jul 2024</t>
   </si>
   <si>
@@ -188,9 +182,21 @@
     <t xml:space="preserve">02 Sep 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">09 Sep 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">16 Sep 2024</t>
   </si>
   <si>
@@ -260,6 +266,12 @@
     <t xml:space="preserve">11 Nov 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 November 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">18 Nov 2024</t>
   </si>
   <si>
@@ -287,7 +299,19 @@
     <t xml:space="preserve">02 Dec 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">09 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">16 Dec 2024</t>
@@ -961,44 +985,36 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7" t="n">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1006,25 +1022,33 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -1038,39 +1062,31 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1078,31 +1094,39 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="n">
         <v>29</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>28</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1110,13 +1134,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1130,19 +1154,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1150,16 +1174,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>30</v>
@@ -1170,16 +1194,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>30</v>
@@ -1190,16 +1214,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>30</v>
@@ -1210,16 +1234,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>30</v>
@@ -1230,13 +1254,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>12</v>
@@ -1250,13 +1274,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1270,16 +1294,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>30</v>
@@ -1290,16 +1314,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>30</v>
@@ -1310,13 +1334,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>12</v>
@@ -1330,51 +1354,51 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1382,16 +1406,16 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>33</v>
@@ -1402,96 +1426,112 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>39</v>
@@ -1502,16 +1542,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>39</v>
@@ -1522,16 +1562,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>39</v>
@@ -1542,92 +1582,92 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>44</v>
@@ -1638,16 +1678,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>44</v>
@@ -1658,16 +1698,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>44</v>
@@ -1678,16 +1718,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>44</v>
@@ -1698,16 +1738,16 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>44</v>
@@ -1718,60 +1758,68 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>47</v>
@@ -1782,19 +1830,19 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1802,16 +1850,16 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>48</v>
@@ -1822,19 +1870,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1842,40 +1890,56 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>51</v>
@@ -1886,16 +1950,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>51</v>
@@ -1906,96 +1970,96 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>5</v>
@@ -2006,16 +2070,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>5</v>
@@ -2026,16 +2090,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>5</v>
@@ -2046,16 +2110,16 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>5</v>
@@ -2066,184 +2130,184 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E72" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E81" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F81" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E82" s="5" t="n">
         <v>17</v>
@@ -2254,16 +2318,16 @@
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E83" s="5" t="n">
         <v>17</v>
@@ -2274,202 +2338,182 @@
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F88" s="5"/>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F89" s="5"/>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F90" s="5"/>
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F91" s="5"/>
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F92" s="5"/>
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F93" s="5"/>
     </row>
     <row r="94">
       <c r="A94" s="5" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F94" s="5"/>
     </row>
     <row r="95">
       <c r="A95" s="5" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F95" s="5"/>
     </row>
     <row r="96">
       <c r="A96" s="5" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F96" s="5"/>
     </row>
     <row r="97">
       <c r="A97" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E97" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E98" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F97" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F98">
+  <conditionalFormatting sqref="A5:F97">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2480,7 +2524,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A98">
+  <conditionalFormatting sqref="A5:A97">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look - weekly update 06.06.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 31 May 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">03 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 June 2024</t>
+    <t xml:space="preserve">10 Jun 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,15 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 June 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">17 Jun 2024</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Justice data lab statistics: July 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2024</t>
   </si>
   <si>
@@ -164,10 +152,13 @@
     <t xml:space="preserve">12 Aug 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 August 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2024</t>
@@ -571,24 +562,24 @@
     <dxf>
       <font>
         <sz val="11"/>
+        <color rgb="FFB4C6E7"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB4C6E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FFB4C6E7"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFB4C6E7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -962,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -972,43 +963,43 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" t="n">
-        <v>25</v>
-      </c>
-      <c r="F7"/>
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1022,13 +1013,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
@@ -1042,51 +1033,51 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1094,13 +1085,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1114,13 +1105,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1134,19 +1125,19 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1154,16 +1145,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>30</v>
@@ -1174,16 +1165,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>30</v>
@@ -1194,16 +1185,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>30</v>
@@ -1214,16 +1205,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>30</v>
@@ -1234,13 +1225,13 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
@@ -1254,13 +1245,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>12</v>
@@ -1274,13 +1265,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1294,16 +1285,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>30</v>
@@ -1314,39 +1305,31 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1356,29 +1339,37 @@
       <c r="A26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1386,16 +1377,16 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>33</v>
@@ -1406,47 +1397,47 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
@@ -1459,10 +1450,10 @@
         <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1472,46 +1463,46 @@
       <c r="A33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>39</v>
@@ -1522,16 +1513,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>39</v>
@@ -1542,16 +1533,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>39</v>
@@ -1562,92 +1553,92 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>44</v>
@@ -1658,16 +1649,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>44</v>
@@ -1678,16 +1669,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>44</v>
@@ -1698,16 +1689,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>44</v>
@@ -1718,16 +1709,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>44</v>
@@ -1738,35 +1729,35 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
@@ -1779,10 +1770,10 @@
         <v>85</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1790,16 +1781,16 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>47</v>
@@ -1810,19 +1801,19 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1830,16 +1821,16 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="C53" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>48</v>
@@ -1850,19 +1841,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1879,10 +1870,10 @@
         <v>96</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1899,10 +1890,10 @@
         <v>99</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1910,16 +1901,16 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>51</v>
@@ -1930,16 +1921,16 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>51</v>
@@ -1950,96 +1941,96 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="C65" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>5</v>
@@ -2050,16 +2041,16 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>5</v>
@@ -2070,16 +2061,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>5</v>
@@ -2090,16 +2081,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>5</v>
@@ -2110,184 +2101,184 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="D76" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="D80" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E80" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F80" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="C81" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E81" s="5" t="n">
         <v>17</v>
@@ -2298,16 +2289,16 @@
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E82" s="5" t="n">
         <v>17</v>
@@ -2318,214 +2309,194 @@
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F88" s="5"/>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F89" s="5"/>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F90" s="5"/>
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F91" s="5"/>
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F92" s="5"/>
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F93" s="5"/>
     </row>
     <row r="94">
       <c r="A94" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F94" s="5"/>
     </row>
     <row r="95">
       <c r="A95" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F95" s="5"/>
     </row>
     <row r="96">
       <c r="A96" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C96" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
+      <c r="D96" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E96" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E97" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F96" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F97">
+  <conditionalFormatting sqref="A5:F96">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A97">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="A5:A96">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>

<commit_message>
Weekly update forward look stats - 14.06.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 June 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 June 2024</t>
+    <t xml:space="preserve">24 Jun 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,18 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 June 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legal aid statistics quarterly: January to March 2024</t>
   </si>
   <si>
@@ -86,34 +74,34 @@
     <t xml:space="preserve">11 July 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">15 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimates of children with a parent in prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimates of children with a parent in prison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Offender Employment Outcomes, update to March 2024</t>
@@ -562,24 +550,24 @@
     <dxf>
       <font>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
         <color rgb="FFB4C6E7"/>
         <name val="Calibri"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD9E1F2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -953,7 +941,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -961,25 +949,33 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F6"/>
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -993,39 +989,31 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1035,29 +1023,37 @@
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1065,13 +1061,13 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -1088,7 +1084,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>27</v>
@@ -1097,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1108,16 +1104,16 @@
         <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1125,13 +1121,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1145,16 +1141,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>30</v>
@@ -1165,13 +1161,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -1185,16 +1181,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>30</v>
@@ -1205,13 +1201,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>12</v>
@@ -1225,13 +1221,13 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
@@ -1245,13 +1241,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>12</v>
@@ -1265,13 +1261,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1285,51 +1281,51 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1337,16 +1333,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>33</v>
@@ -1357,16 +1353,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>33</v>
@@ -1377,63 +1373,63 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1441,48 +1437,48 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>39</v>
@@ -1493,16 +1489,16 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>39</v>
@@ -1513,16 +1509,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>39</v>
@@ -1533,92 +1529,92 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>44</v>
@@ -1629,16 +1625,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C43" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>44</v>
@@ -1649,16 +1645,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>44</v>
@@ -1669,16 +1665,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>44</v>
@@ -1689,16 +1685,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>44</v>
@@ -1709,51 +1705,51 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1761,16 +1757,16 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>47</v>
@@ -1784,16 +1780,16 @@
         <v>83</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1801,16 +1797,16 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>48</v>
@@ -1824,16 +1820,16 @@
         <v>87</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1841,19 +1837,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1861,19 +1857,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1881,16 +1877,16 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>51</v>
@@ -1901,16 +1897,16 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>51</v>
@@ -1921,96 +1917,96 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>5</v>
@@ -2021,16 +2017,16 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="C65" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>5</v>
@@ -2041,16 +2037,16 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>5</v>
@@ -2061,16 +2057,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>5</v>
@@ -2081,184 +2077,184 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E79" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F79" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E80" s="5" t="n">
         <v>17</v>
@@ -2269,16 +2265,16 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="C81" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E81" s="5" t="n">
         <v>17</v>
@@ -2289,214 +2285,194 @@
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F88" s="5"/>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F89" s="5"/>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F90" s="5"/>
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F91" s="5"/>
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F92" s="5"/>
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F93" s="5"/>
     </row>
     <row r="94">
       <c r="A94" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F94" s="5"/>
     </row>
     <row r="95">
       <c r="A95" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E95" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F95" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F96">
+  <conditionalFormatting sqref="A5:F95">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A96">
-    <cfRule type="expression" dxfId="1" priority="4">
+  <conditionalFormatting sqref="A5:A95">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="2">

</xml_diff>

<commit_message>
forward look weekly update 21.06.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 June 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -101,42 +101,42 @@
     <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Offender Employment Outcomes, update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: July 2022 to September 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community Performance Annual, update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMPPS Annual Digest, April 2023 to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June with 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 August 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">Offender Employment Outcomes, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: July 2022 to September 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community Performance Annual, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMPPS Annual Digest, April 2023 to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June with 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 August 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">12 Aug 2024</t>
   </si>
   <si>
@@ -170,34 +170,34 @@
     <t xml:space="preserve">09 Sep 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">16 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Sep 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tribunals statistics quarterly: April to June 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">12 September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 Sep 2024</t>
+    <t xml:space="preserve">3 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">07 Oct 2024</t>
@@ -1110,7 +1110,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>30</v>
@@ -1124,7 +1124,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>27</v>
@@ -1144,7 +1144,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>27</v>
@@ -1164,7 +1164,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>27</v>
@@ -1184,7 +1184,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>27</v>
@@ -1204,7 +1204,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>27</v>
@@ -1244,7 +1244,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>27</v>
@@ -1264,7 +1264,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>27</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1293,16 +1293,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>32</v>
@@ -1322,7 +1322,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>33</v>
@@ -1362,7 +1362,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>33</v>
@@ -1406,7 +1406,7 @@
         <v>50</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>36</v>
@@ -1419,25 +1419,17 @@
       <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1449,16 +1441,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>39</v>
@@ -1469,16 +1461,16 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>39</v>
@@ -1489,16 +1481,16 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>39</v>
@@ -1509,16 +1501,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D36" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>39</v>
@@ -1529,15 +1521,23 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E37" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
@@ -1562,7 +1562,7 @@
         <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>42</v>
@@ -1594,7 +1594,7 @@
         <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>44</v>
@@ -1614,7 +1614,7 @@
         <v>69</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>44</v>
@@ -1634,7 +1634,7 @@
         <v>69</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>44</v>
@@ -1654,7 +1654,7 @@
         <v>69</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>44</v>
@@ -1674,7 +1674,7 @@
         <v>69</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>44</v>
@@ -1694,7 +1694,7 @@
         <v>69</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>44</v>
@@ -1726,7 +1726,7 @@
         <v>78</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>46</v>
@@ -1746,7 +1746,7 @@
         <v>81</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>47</v>
@@ -1786,7 +1786,7 @@
         <v>85</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>48</v>
@@ -1806,7 +1806,7 @@
         <v>85</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>48</v>
@@ -1826,7 +1826,7 @@
         <v>89</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>49</v>
@@ -1846,7 +1846,7 @@
         <v>92</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>50</v>
@@ -1866,7 +1866,7 @@
         <v>95</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>51</v>
@@ -1886,7 +1886,7 @@
         <v>95</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>51</v>
@@ -1906,7 +1906,7 @@
         <v>95</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>51</v>
@@ -1986,7 +1986,7 @@
         <v>105</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>5</v>
@@ -2006,7 +2006,7 @@
         <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>5</v>
@@ -2026,7 +2026,7 @@
         <v>105</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>5</v>
@@ -2046,7 +2046,7 @@
         <v>105</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>5</v>
@@ -2066,7 +2066,7 @@
         <v>105</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>5</v>
@@ -2110,7 +2110,7 @@
         <v>114</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>8</v>
@@ -2178,7 +2178,7 @@
         <v>121</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>13</v>
@@ -2234,7 +2234,7 @@
         <v>127</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E79" s="5" t="n">
         <v>17</v>
@@ -2254,7 +2254,7 @@
         <v>127</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E80" s="5" t="n">
         <v>17</v>
@@ -2274,7 +2274,7 @@
         <v>127</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E81" s="5" t="n">
         <v>17</v>
@@ -2450,7 +2450,7 @@
         <v>145</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E95" s="5" t="n">
         <v>31</v>

</xml_diff>

<commit_message>
weekly forward look update 28.06.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 June 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">24 Jun 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 June 2024</t>
+    <t xml:space="preserve">08 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,24 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 July 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">15 Jul 2024</t>
   </si>
   <si>
@@ -365,6 +347,12 @@
     <t xml:space="preserve">03 Mar 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 March 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 Mar 2025</t>
   </si>
   <si>
@@ -411,6 +399,12 @@
   </si>
   <si>
     <t xml:space="preserve">12 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">19 May 2025</t>
@@ -574,6 +568,18 @@
     <dxf>
       <font>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color rgb="FFFFFFFF"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
         <color rgb="FFD9E1F2"/>
         <name val="Calibri"/>
       </font>
@@ -582,18 +588,6 @@
           <bgColor rgb="FFD9E1F2"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color rgb="FFFFFFFF"/>
-        </top>
-      </border>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -941,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -949,19 +943,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -969,19 +963,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -989,31 +983,39 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" t="n">
-        <v>27</v>
-      </c>
-      <c r="F8"/>
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1021,19 +1023,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -1041,19 +1043,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1061,19 +1063,19 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1081,13 +1083,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1101,13 +1103,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1121,13 +1123,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1141,13 +1143,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1161,13 +1163,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -1181,13 +1183,13 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>12</v>
@@ -1201,39 +1203,31 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1241,19 +1235,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1261,19 +1255,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1281,71 +1275,63 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1353,23 +1339,15 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
@@ -1379,7 +1357,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1387,29 +1365,37 @@
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D30" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1417,27 +1403,43 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
@@ -1450,10 +1452,10 @@
         <v>55</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="5" t="n">
         <v>40</v>
-      </c>
-      <c r="E33" s="5" t="n">
-        <v>39</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1461,39 +1463,31 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1501,39 +1495,31 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1541,31 +1527,39 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1573,28 +1567,36 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>44</v>
@@ -1605,16 +1607,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>44</v>
@@ -1625,39 +1627,31 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1665,19 +1659,19 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1685,19 +1679,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1705,31 +1699,39 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1737,19 +1739,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1757,19 +1759,19 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1777,19 +1779,19 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1797,19 +1799,19 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1820,16 +1822,16 @@
         <v>87</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>89</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1837,156 +1839,156 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="C61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="C62" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="C63" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>5</v>
@@ -1997,59 +1999,43 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="D66" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -2057,131 +2043,131 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B67" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="B68" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C70" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="B71" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E75" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>13</v>
@@ -2189,75 +2175,83 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+        <v>121</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E80" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>13</v>
@@ -2265,217 +2259,161 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F88" s="5"/>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F89" s="5"/>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F90" s="5"/>
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E91" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E95" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F91" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F95">
+  <conditionalFormatting sqref="A5:F91">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="4">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A95">
+  <conditionalFormatting sqref="A5:A91">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1,$E5=$E4)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
weekly update stats forward look 03.07.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 June 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 03 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -568,6 +568,18 @@
     <dxf>
       <font>
         <sz val="11"/>
+        <color rgb="FFD9E1F2"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
       </font>
@@ -576,18 +588,6 @@
           <color rgb="FFFFFFFF"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FFD9E1F2"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -2405,7 +2405,7 @@
     <cfRule type="expression" dxfId="1" priority="4">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2413,7 +2413,7 @@
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1,$E5=$E4)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
weekly stats forward look update 12.07.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 03 July 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,28 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">08 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2024 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 July 2024</t>
+    <t xml:space="preserve">15 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
@@ -935,7 +926,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -943,13 +934,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -963,13 +954,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -983,19 +974,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1003,13 +994,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
@@ -1023,13 +1014,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -1043,13 +1034,13 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -1063,13 +1054,13 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -1083,13 +1074,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1103,13 +1094,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1123,13 +1114,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1143,13 +1134,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1163,13 +1154,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -1183,51 +1174,51 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <v>33</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>32</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1235,16 +1226,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>33</v>
@@ -1255,13 +1246,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1275,104 +1266,104 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>39</v>
@@ -1383,16 +1374,16 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>39</v>
@@ -1403,16 +1394,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>39</v>
@@ -1423,19 +1414,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1445,78 +1436,78 @@
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>44</v>
@@ -1527,16 +1518,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>44</v>
@@ -1547,16 +1538,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>44</v>
@@ -1567,16 +1558,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>44</v>
@@ -1587,16 +1578,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>44</v>
@@ -1607,35 +1598,35 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
@@ -1648,10 +1639,10 @@
         <v>72</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1659,16 +1650,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C45" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>47</v>
@@ -1679,19 +1670,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1699,16 +1690,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>48</v>
@@ -1719,19 +1710,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1748,10 +1739,10 @@
         <v>83</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1768,10 +1759,10 @@
         <v>86</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1779,16 +1770,16 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>51</v>
@@ -1799,16 +1790,16 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>51</v>
@@ -1819,96 +1810,96 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C53" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>5</v>
@@ -1919,16 +1910,16 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>5</v>
@@ -1939,16 +1930,16 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>5</v>
@@ -1959,16 +1950,16 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>5</v>
@@ -1979,192 +1970,192 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="D70" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="D74" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E74" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F74" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="C75" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>17</v>
@@ -2175,16 +2166,16 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E76" s="5" t="n">
         <v>17</v>
@@ -2195,210 +2186,190 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C77" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="D79" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E79" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F79" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F88" s="5"/>
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F89" s="5"/>
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
+      <c r="D90" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E90" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E91" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F91" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F91">
+  <conditionalFormatting sqref="A5:F90">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2409,7 +2380,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A91">
+  <conditionalFormatting sqref="A5:A90">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 19.07.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 12 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 19 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.gov.uk/search/research-and-statistics?content_store_document_type=upcoming_statistics&amp;organisations%5B%5D=ministry-of-justice&amp;order=release-date-oldest</t>
   </si>
   <si>
     <t xml:space="preserve">Week Commencing</t>
@@ -41,34 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">15 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 July 2024</t>
+    <t xml:space="preserve">22 Jul 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Annual Statistics Publication, England and Wales: April 2023 to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimates of children with a parent in prison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 July 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
@@ -442,7 +427,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -466,12 +451,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <u val="single"/>
     </font>
     <font>
       <sz val="11"/>
@@ -509,10 +488,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -870,7 +849,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="96.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="79.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
@@ -926,7 +905,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -946,7 +925,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -966,7 +945,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -974,13 +953,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -994,13 +973,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
@@ -1014,13 +993,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -1034,13 +1013,13 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -1054,13 +1033,13 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -1074,13 +1053,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1094,13 +1073,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1114,39 +1093,31 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1154,19 +1125,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1176,29 +1147,37 @@
       <c r="A18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1208,57 +1187,41 @@
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1272,7 +1235,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F23" s="5"/>
     </row>
@@ -1284,7 +1247,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -1299,10 +1262,10 @@
         <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1310,40 +1273,56 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>39</v>
@@ -1354,19 +1333,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1374,39 +1353,31 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1414,51 +1385,51 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1466,28 +1437,36 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>44</v>
@@ -1498,16 +1477,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>44</v>
@@ -1518,16 +1497,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>44</v>
@@ -1538,39 +1517,31 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="D40" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1578,19 +1549,19 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1598,31 +1569,39 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1630,19 +1609,19 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1650,19 +1629,19 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1670,19 +1649,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1690,19 +1669,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1710,19 +1689,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1730,19 +1709,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1752,134 +1731,134 @@
       <c r="A50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>5</v>
@@ -1890,16 +1869,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>5</v>
@@ -1910,59 +1889,43 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D62" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1976,7 +1939,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F63" s="5"/>
     </row>
@@ -1984,33 +1947,33 @@
       <c r="A64" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C65" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
@@ -2020,7 +1983,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -2035,10 +1998,10 @@
         <v>109</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -2052,7 +2015,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F68" s="5"/>
     </row>
@@ -2064,7 +2027,7 @@
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F69" s="5"/>
     </row>
@@ -2072,113 +2035,113 @@
       <c r="A70" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E72" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F72" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>13</v>
@@ -2192,7 +2155,7 @@
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F77" s="5"/>
     </row>
@@ -2204,7 +2167,7 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F78" s="5"/>
     </row>
@@ -2212,164 +2175,120 @@
       <c r="A79" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F81" s="5"/>
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F82" s="5"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F83" s="5"/>
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F84" s="5"/>
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="D87" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E87" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F87" s="5"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D90" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E90" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F90" s="5" t="s">
+      <c r="F87" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F90">
+  <conditionalFormatting sqref="A5:F87">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2380,7 +2299,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A90">
+  <conditionalFormatting sqref="A5:A87">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
@@ -2388,9 +2307,6 @@
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1,$E5=$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1h"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
weekly stats forward look update 26.07.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 19 July 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gov.uk/search/research-and-statistics?content_store_document_type=upcoming_statistics&amp;organisations%5B%5D=ministry-of-justice&amp;order=release-date-oldest</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 26 July 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
   </si>
   <si>
     <t xml:space="preserve">Week Commencing</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">22 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Performance Ratings: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 July 2024</t>
+    <t xml:space="preserve">05 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,75 +56,39 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender Employment Outcomes, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: July 2022 to September 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community Performance Annual, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMPPS Annual Digest, April 2023 to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Jul 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June with 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 August 2024</t>
+    <t xml:space="preserve">12 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 August 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">12 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 August 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 September 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">09 Sep 2024</t>
   </si>
   <si>
@@ -162,12 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">14 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Monitoring Statistics Quarterly Publication, September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">21 Oct 2024</t>
@@ -427,7 +385,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -451,6 +409,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <u val="single"/>
     </font>
     <font>
       <sz val="11"/>
@@ -488,10 +452,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -905,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -913,19 +877,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -933,19 +897,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -953,19 +917,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -973,59 +937,43 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1033,59 +981,43 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1093,31 +1025,39 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1128,16 +1068,16 @@
         <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1145,19 +1085,19 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1165,63 +1105,55 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1229,43 +1161,59 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1276,16 +1224,16 @@
         <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1296,16 +1244,16 @@
         <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1313,39 +1261,31 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="5" t="n">
         <v>46</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>40</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1353,31 +1293,39 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1385,31 +1333,39 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1417,19 +1373,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1437,19 +1393,19 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1457,19 +1413,19 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1477,19 +1433,19 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1497,19 +1453,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1517,111 +1473,79 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1629,19 +1553,19 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1649,19 +1573,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1669,19 +1593,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1689,19 +1613,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1709,119 +1633,119 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1829,103 +1753,95 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1933,362 +1849,190 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B71" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="E71" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F78" s="5"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F82" s="5"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E87" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F87">
+  <conditionalFormatting sqref="A5:F76">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2299,7 +2043,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A87">
+  <conditionalFormatting sqref="A5:A76">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>
@@ -2307,6 +2051,9 @@
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=1,$E5=$E4)</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1h"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
weekly stats forward look update 08.08.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 02 August 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">11 Nov 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2023</t>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">14 November 2024</t>

</xml_diff>

<commit_message>
weekly forward look stats update 14.08.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 August 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,28 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">05 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 August 2024</t>
+    <t xml:space="preserve">12 Aug 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
@@ -869,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -877,13 +868,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -897,13 +888,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -917,104 +908,104 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>39</v>
@@ -1025,16 +1016,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>39</v>
@@ -1045,16 +1036,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>39</v>
@@ -1065,19 +1056,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1087,70 +1078,70 @@
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>44</v>
@@ -1161,16 +1152,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>44</v>
@@ -1181,16 +1172,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>44</v>
@@ -1201,16 +1192,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>44</v>
@@ -1221,16 +1212,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>44</v>
@@ -1241,35 +1232,35 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
@@ -1282,10 +1273,10 @@
         <v>50</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1293,16 +1284,16 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>47</v>
@@ -1313,19 +1304,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1333,16 +1324,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>48</v>
@@ -1353,19 +1344,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1382,10 +1373,10 @@
         <v>61</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1402,10 +1393,10 @@
         <v>64</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1413,16 +1404,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>51</v>
@@ -1433,16 +1424,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>51</v>
@@ -1453,96 +1444,96 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C44" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>5</v>
@@ -1553,16 +1544,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>5</v>
@@ -1573,16 +1564,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>5</v>
@@ -1593,16 +1584,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>5</v>
@@ -1613,192 +1604,192 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="C60" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>17</v>
@@ -1809,16 +1800,16 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>17</v>
@@ -1829,210 +1820,190 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F75" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F76">
+  <conditionalFormatting sqref="A5:F75">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2043,7 +2014,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A76">
+  <conditionalFormatting sqref="A5:A75">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats weekly forward look update 23.08.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 August 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 23 August 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">12 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 August 2024</t>
+    <t xml:space="preserve">02 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,46 +56,25 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics: January to March 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 Aug 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 September 2024</t>
+    <t xml:space="preserve">09 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
@@ -860,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -868,83 +847,83 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7" t="n">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" t="n">
-        <v>34</v>
-      </c>
-      <c r="F8"/>
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -952,103 +931,95 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1056,19 +1027,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1076,52 +1047,76 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>44</v>
@@ -1132,39 +1127,31 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1172,19 +1159,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1192,19 +1179,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1212,19 +1199,19 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1232,31 +1219,39 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1264,19 +1259,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="5" t="n">
         <v>50</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>47</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1284,19 +1279,19 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="5" t="n">
         <v>51</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>47</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1304,19 +1299,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1324,19 +1319,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1344,219 +1339,203 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1564,39 +1543,31 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1604,43 +1575,43 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1648,35 +1619,27 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
@@ -1686,7 +1649,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -1694,29 +1657,37 @@
       <c r="A54" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="B54" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1724,15 +1695,23 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
@@ -1742,7 +1721,7 @@
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F57" s="5"/>
     </row>
@@ -1754,7 +1733,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -1769,10 +1748,10 @@
         <v>98</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>13</v>
@@ -1780,43 +1759,27 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="5" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="E60" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
@@ -1826,7 +1789,7 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -1838,7 +1801,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F63" s="5"/>
     </row>
@@ -1846,164 +1809,96 @@
       <c r="A64" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="D70" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F70" s="5"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F72" s="5"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F70" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F75">
+  <conditionalFormatting sqref="A5:F70">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2014,7 +1909,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A75">
+  <conditionalFormatting sqref="A5:A70">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 06.09
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 30 August 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,34 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">02 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 September 2024</t>
+    <t xml:space="preserve">23 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
@@ -839,7 +824,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -847,40 +832,56 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
       <c r="E6" t="n">
-        <v>37</v>
-      </c>
-      <c r="F6"/>
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" t="n">
-        <v>38</v>
-      </c>
-      <c r="F7"/>
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E8" t="n">
         <v>39</v>
@@ -891,19 +892,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -911,112 +912,112 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>44</v>
@@ -1027,16 +1028,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>44</v>
@@ -1047,16 +1048,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>44</v>
@@ -1067,39 +1068,31 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1107,19 +1100,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1127,31 +1120,39 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E22" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1159,19 +1160,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1179,19 +1180,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1199,19 +1200,19 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1219,19 +1220,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1239,19 +1240,19 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="5" t="n">
         <v>51</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>49</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1259,19 +1260,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1281,134 +1282,134 @@
       <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>5</v>
@@ -1419,16 +1420,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>5</v>
@@ -1439,59 +1440,43 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1505,7 +1490,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1513,33 +1498,33 @@
       <c r="A44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
@@ -1549,7 +1534,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -1564,10 +1549,10 @@
         <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1581,7 +1566,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -1593,7 +1578,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1601,113 +1586,113 @@
       <c r="A50" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="D56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="5" t="n">
         <v>20</v>
-      </c>
-      <c r="E56" s="5" t="n">
-        <v>17</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1721,7 +1706,7 @@
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F57" s="5"/>
     </row>
@@ -1733,7 +1718,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -1741,164 +1726,120 @@
       <c r="A59" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F68" s="5"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F69" s="5"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F67" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F70">
+  <conditionalFormatting sqref="A5:F67">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1909,7 +1850,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A70">
+  <conditionalFormatting sqref="A5:A67">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly stats forward look update 13.09.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 September 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -59,13 +59,13 @@
     <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">30 Sep 2024</t>
@@ -841,7 +841,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
         <v>39</v>
@@ -855,7 +855,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -875,13 +875,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
         <v>39</v>
@@ -957,7 +957,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>44</v>
@@ -977,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>44</v>
@@ -997,7 +997,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>44</v>
@@ -1017,7 +1017,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>44</v>
@@ -1037,7 +1037,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>44</v>
@@ -1057,7 +1057,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>44</v>
@@ -1089,7 +1089,7 @@
         <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>46</v>
@@ -1109,7 +1109,7 @@
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>47</v>
@@ -1149,7 +1149,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>48</v>
@@ -1169,7 +1169,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>48</v>
@@ -1189,7 +1189,7 @@
         <v>46</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>49</v>
@@ -1209,7 +1209,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>50</v>
@@ -1229,7 +1229,7 @@
         <v>52</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>51</v>
@@ -1249,7 +1249,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>51</v>
@@ -1269,7 +1269,7 @@
         <v>52</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>51</v>
@@ -1349,7 +1349,7 @@
         <v>62</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>5</v>
@@ -1369,7 +1369,7 @@
         <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>5</v>
@@ -1389,7 +1389,7 @@
         <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>5</v>
@@ -1409,7 +1409,7 @@
         <v>62</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>5</v>
@@ -1429,7 +1429,7 @@
         <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>5</v>
@@ -1473,7 +1473,7 @@
         <v>71</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>8</v>
@@ -1505,7 +1505,7 @@
         <v>75</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>10</v>
@@ -1549,7 +1549,7 @@
         <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13</v>
@@ -1605,7 +1605,7 @@
         <v>86</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>17</v>
@@ -1625,7 +1625,7 @@
         <v>86</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>17</v>
@@ -1645,7 +1645,7 @@
         <v>86</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>17</v>
@@ -1689,7 +1689,7 @@
         <v>93</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>20</v>
@@ -1829,7 +1829,7 @@
         <v>106</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>31</v>

</xml_diff>

<commit_message>
weekly forward look stats update 20.09.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 September 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 20 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -977,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>44</v>
@@ -1017,7 +1017,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>44</v>
@@ -1037,7 +1037,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>44</v>
@@ -1057,7 +1057,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
weekly forward look stats update 27.09.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 20 September 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 27 September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">23 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Education and Accredited Programme Statistics 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 September 2024</t>
+    <t xml:space="preserve">30 Sep 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,51 +56,33 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: April - June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: April - June 2024</t>
+    <t xml:space="preserve">07 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">30 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 October 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 October 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">Offender management statistics quarterly: April to June 2024 </t>
   </si>
   <si>
@@ -125,12 +107,15 @@
     <t xml:space="preserve">18 Nov 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 November 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">21 November 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2024</t>
   </si>
   <si>
@@ -209,6 +194,9 @@
     <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
   </si>
   <si>
+    <t xml:space="preserve">Justice data lab statistics: January 2025.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
   </si>
   <si>
@@ -230,6 +218,9 @@
     <t xml:space="preserve">20 February 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 Feb 2025</t>
   </si>
   <si>
@@ -257,6 +248,9 @@
     <t xml:space="preserve">27 March 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 Mar 2025</t>
   </si>
   <si>
@@ -275,6 +269,9 @@
     <t xml:space="preserve">24 April 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
   </si>
   <si>
@@ -287,6 +284,12 @@
     <t xml:space="preserve">05 May 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Coroners statistics 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 May 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">12 May 2025</t>
   </si>
   <si>
@@ -296,6 +299,18 @@
     <t xml:space="preserve">13 May 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">19 May 2025</t>
   </si>
   <si>
@@ -320,6 +335,12 @@
     <t xml:space="preserve">07 Jul 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 July 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">14 Jul 2025</t>
   </si>
   <si>
@@ -329,10 +350,19 @@
     <t xml:space="preserve">28 Jul 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 July 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: January 2025 to March 2025 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">31 July 2025</t>
+    <t xml:space="preserve">Prison Performance Ratings: 2024 to 2025</t>
   </si>
 </sst>
 </file>
@@ -768,7 +798,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="79.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="108.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
@@ -824,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -832,79 +862,55 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7" t="n">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -912,49 +918,73 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -968,13 +998,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -988,39 +1018,31 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1028,19 +1050,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1048,19 +1070,19 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1068,31 +1090,39 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1100,19 +1130,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1120,19 +1150,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1140,19 +1170,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1160,19 +1190,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1180,19 +1210,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1200,19 +1230,19 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1222,134 +1252,134 @@
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="n">
         <v>52</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>5</v>
@@ -1360,16 +1390,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>5</v>
@@ -1380,16 +1410,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>5</v>
@@ -1400,156 +1430,156 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13</v>
@@ -1560,7 +1590,7 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1572,7 +1602,7 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1584,7 +1614,7 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1596,16 +1626,16 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>17</v>
@@ -1616,16 +1646,16 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>17</v>
@@ -1636,16 +1666,16 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="D53" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>17</v>
@@ -1656,43 +1686,51 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1700,146 +1738,294 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" s="5" t="n">
+      <c r="B68" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F67">
+  <conditionalFormatting sqref="A5:F74">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1850,7 +2036,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A67">
+  <conditionalFormatting sqref="A5:A74">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 04.10.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 27 September 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 04 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,31 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">30 Sep 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 October 2024</t>
+    <t xml:space="preserve">14 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An ad-hoc statistical publication containing statistics on the number of Welsh speaking prisoners recorded across English and Welsh estates, and number of Welsh speaking people on probation from 2020 onwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad-hoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,31 +74,13 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">07 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 October 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
   </si>
   <si>
     <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">provisional</t>
+    <t xml:space="preserve">Unpaid Work Management Information, update to June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Offender management statistics quarterly: April to June 2024 </t>
@@ -329,6 +329,12 @@
     <t xml:space="preserve">23 Jun 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 June 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 Jun 2025</t>
   </si>
   <si>
@@ -363,6 +369,45 @@
   </si>
   <si>
     <t xml:space="preserve">Prison Performance Ratings: 2024 to 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 Aug 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Aug 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Aug 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 August 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Aug 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 Sep 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 Sep 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Sep 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Sep 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: April to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 September 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: April to June 2025</t>
   </si>
 </sst>
 </file>
@@ -798,7 +843,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="108.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="207.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
@@ -854,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -868,7 +913,7 @@
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6"/>
     </row>
@@ -876,55 +921,71 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" t="n">
-        <v>42</v>
-      </c>
-      <c r="F7"/>
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" t="n">
-        <v>43</v>
-      </c>
-      <c r="F8"/>
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -933,119 +994,119 @@
         <v>44</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -1053,19 +1114,19 @@
         <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>47</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -1073,39 +1134,39 @@
         <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>47</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -1113,79 +1174,79 @@
         <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
@@ -1193,19 +1254,19 @@
         <v>45</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
@@ -1213,119 +1274,119 @@
         <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>51</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33">
@@ -1333,19 +1394,19 @@
         <v>55</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
@@ -1353,19 +1414,19 @@
         <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
@@ -1373,19 +1434,19 @@
         <v>55</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36">
@@ -1393,255 +1454,255 @@
         <v>55</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52">
@@ -1649,19 +1710,19 @@
         <v>82</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -1669,71 +1730,71 @@
         <v>82</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57">
@@ -1741,19 +1802,19 @@
         <v>92</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58">
@@ -1761,19 +1822,19 @@
         <v>92</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59">
@@ -1781,251 +1842,371 @@
         <v>92</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E71" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E72" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="D73" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E73" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F74">
+  <conditionalFormatting sqref="A5:F82">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2036,7 +2217,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A74">
+  <conditionalFormatting sqref="A5:A82">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 11.10.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 04 October 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 11 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -1100,7 +1100,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>47</v>
@@ -1120,7 +1120,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>47</v>

</xml_diff>

<commit_message>
weekly stats forward look update 18.10.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 11 October 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 18 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,46 +41,34 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">14 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An ad-hoc statistical publication containing statistics on the number of Welsh speaking prisoners recorded across English and Welsh estates, and number of Welsh speaking people on probation from 2020 onwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 October 2024</t>
+    <t xml:space="preserve">28 Oct 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unpaid Work Management Information, update to June 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 October 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unpaid Work Management Information, update to June 2024</t>
+    <t xml:space="preserve">Turnaround Programme: Management Information, January – December 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Offender management statistics quarterly: April to June 2024 </t>
@@ -843,7 +831,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="207.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="108.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
@@ -899,7 +887,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -907,85 +895,93 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" t="n">
-        <v>43</v>
-      </c>
-      <c r="F6"/>
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -994,179 +990,179 @@
         <v>44</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>44</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>47</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>47</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>48</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -1174,70 +1170,70 @@
         <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
@@ -1246,967 +1242,947 @@
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C24" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>5</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>8</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>17</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D57" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D58" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>20</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E66" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="C71" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E71" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E72" s="5" t="n">
         <v>31</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C73" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+        <v>124</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E80" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F80" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E81" s="5" t="n">
         <v>39</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F82">
+  <conditionalFormatting sqref="A5:F81">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2217,7 +2193,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A82">
+  <conditionalFormatting sqref="A5:A81">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 25.10.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 18 October 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 25 October 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -68,6 +68,9 @@
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
+    <t xml:space="preserve">Transparency Data: End of Custody Supervised Licence (ECSL) data, Oct 2023 to Sep 2024 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Turnaround Programme: Management Information, January – December 2023</t>
   </si>
   <si>
@@ -396,6 +399,30 @@
   </si>
   <si>
     <t xml:space="preserve">Legal aid statistics quarterly: April to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Sep 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Oct 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Oct 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Oct 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Oct 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 October 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2024/2025</t>
   </si>
 </sst>
 </file>
@@ -964,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>44</v>
@@ -1035,51 +1062,51 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1087,13 +1114,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1107,13 +1134,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -1127,19 +1154,19 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1147,16 +1174,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>48</v>
@@ -1167,19 +1194,19 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1187,19 +1214,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1207,19 +1234,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1227,16 +1254,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>51</v>
@@ -1247,16 +1274,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>51</v>
@@ -1267,15 +1294,23 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
@@ -1285,7 +1320,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -1297,7 +1332,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -1309,7 +1344,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1321,7 +1356,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="5"/>
     </row>
@@ -1329,31 +1364,23 @@
       <c r="A30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>17</v>
@@ -1367,13 +1394,13 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>17</v>
@@ -1387,13 +1414,13 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>17</v>
@@ -1407,13 +1434,13 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>17</v>
@@ -1427,13 +1454,13 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>17</v>
@@ -1447,15 +1474,23 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
@@ -1465,7 +1500,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -1473,31 +1508,23 @@
       <c r="A38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>17</v>
@@ -1511,47 +1538,55 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
@@ -1561,7 +1596,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1569,31 +1604,23 @@
       <c r="A44" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>17</v>
@@ -1607,15 +1634,23 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
@@ -1625,7 +1660,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -1637,7 +1672,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -1645,31 +1680,23 @@
       <c r="A49" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>17</v>
@@ -1683,13 +1710,13 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>17</v>
@@ -1703,13 +1730,13 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>17</v>
@@ -1723,51 +1750,51 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="D55" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1775,13 +1802,13 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>17</v>
@@ -1795,13 +1822,13 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>17</v>
@@ -1815,13 +1842,13 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>17</v>
@@ -1835,15 +1862,23 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
@@ -1853,7 +1888,7 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -1865,7 +1900,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F61" s="5"/>
     </row>
@@ -1877,7 +1912,7 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -1889,7 +1924,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F63" s="5"/>
     </row>
@@ -1897,65 +1932,65 @@
       <c r="A64" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
@@ -1965,7 +2000,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F68" s="5"/>
     </row>
@@ -1973,31 +2008,23 @@
       <c r="A69" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>17</v>
@@ -2011,13 +2038,13 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>17</v>
@@ -2031,13 +2058,13 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>17</v>
@@ -2051,15 +2078,23 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
@@ -2069,7 +2104,7 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F74" s="5"/>
     </row>
@@ -2077,33 +2112,33 @@
       <c r="A75" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="D76" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
@@ -2113,7 +2148,7 @@
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F77" s="5"/>
     </row>
@@ -2125,7 +2160,7 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F78" s="5"/>
     </row>
@@ -2137,7 +2172,7 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F79" s="5"/>
     </row>
@@ -2145,31 +2180,23 @@
       <c r="A80" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
       <c r="E80" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F80" s="5"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B81" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>17</v>
@@ -2181,8 +2208,116 @@
         <v>13</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F81">
+  <conditionalFormatting sqref="A5:F88">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2193,7 +2328,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A81">
+  <conditionalFormatting sqref="A5:A88">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 01.11.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 25 October 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 01 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,69 +41,33 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">28 Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 October 2024</t>
+    <t xml:space="preserve">11 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2023/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: October 2022 to December 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unpaid Work Management Information, update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transparency Data: End of Custody Supervised Licence (ECSL) data, Oct 2023 to Sep 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turnaround Programme: Management Information, January – December 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: April to June 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: October 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 November 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 November 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
   </si>
   <si>
@@ -320,12 +284,15 @@
     <t xml:space="preserve">23 Jun 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 June 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">26 June 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">30 Jun 2025</t>
   </si>
   <si>
@@ -368,6 +335,12 @@
     <t xml:space="preserve">11 Aug 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics:  April to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 August 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">18 Aug 2025</t>
   </si>
   <si>
@@ -383,6 +356,12 @@
     <t xml:space="preserve">01 Sep 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: April to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 September 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">08 Sep 2025</t>
   </si>
   <si>
@@ -420,6 +399,9 @@
   </si>
   <si>
     <t xml:space="preserve">30 October 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: October to December 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2024/2025</t>
@@ -914,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -922,19 +904,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -942,19 +924,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -962,19 +944,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -982,19 +964,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1002,19 +984,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -1022,19 +1004,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1042,19 +1024,19 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1062,19 +1044,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1082,31 +1064,39 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1114,119 +1104,79 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1234,19 +1184,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1254,19 +1204,19 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1274,19 +1224,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1294,19 +1244,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1314,15 +1264,23 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
@@ -1332,7 +1290,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -1344,7 +1302,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1352,61 +1310,69 @@
       <c r="A29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1414,59 +1380,43 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1474,19 +1424,19 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1494,63 +1444,55 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="5" t="n">
         <v>17</v>
-      </c>
-      <c r="E40" s="5" t="n">
-        <v>8</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1558,31 +1500,39 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="5" t="n">
         <v>17</v>
-      </c>
-      <c r="E42" s="5" t="n">
-        <v>10</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1590,43 +1540,51 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1634,19 +1592,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1654,147 +1612,139 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1805,16 +1755,16 @@
         <v>89</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>91</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1822,39 +1772,31 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
@@ -1862,131 +1804,155 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E66" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -1994,83 +1960,75 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>13</v>
@@ -2078,19 +2036,19 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>13</v>
@@ -2098,226 +2056,114 @@
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F77" s="5"/>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E78" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F78" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E79" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F79" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+        <v>126</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E80" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E81" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="F87" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E88" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F88" s="5" t="s">
+      <c r="F80" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F88">
+  <conditionalFormatting sqref="A5:F80">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2328,7 +2174,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A88">
+  <conditionalFormatting sqref="A5:A80">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats weekly forward look update 08.11.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 01 November 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -50,40 +50,40 @@
     <t xml:space="preserve">14 November 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2023 to 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 November 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 November 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2023 to 2024</t>
   </si>
   <si>
     <t xml:space="preserve">02 Dec 2024</t>
@@ -913,7 +913,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
         <v>47</v>
@@ -927,13 +927,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
         <v>47</v>
@@ -947,13 +947,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
         <v>47</v>
@@ -964,16 +964,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>48</v>
@@ -984,16 +984,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>48</v>
@@ -1013,7 +1013,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>49</v>
@@ -1033,7 +1033,7 @@
         <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>50</v>
@@ -1053,7 +1053,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>51</v>
@@ -1073,7 +1073,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>51</v>
@@ -1093,7 +1093,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>51</v>
@@ -1173,7 +1173,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>5</v>
@@ -1193,7 +1193,7 @@
         <v>42</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>5</v>
@@ -1213,7 +1213,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>5</v>
@@ -1233,7 +1233,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>5</v>
@@ -1253,7 +1253,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>5</v>
@@ -1273,7 +1273,7 @@
         <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>5</v>
@@ -1317,7 +1317,7 @@
         <v>52</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>8</v>
@@ -1337,7 +1337,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>8</v>
@@ -1369,7 +1369,7 @@
         <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>10</v>
@@ -1413,7 +1413,7 @@
         <v>62</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13</v>
@@ -1433,7 +1433,7 @@
         <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13</v>
@@ -1489,7 +1489,7 @@
         <v>69</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>17</v>
@@ -1509,7 +1509,7 @@
         <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>17</v>
@@ -1529,7 +1529,7 @@
         <v>69</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>17</v>
@@ -1549,7 +1549,7 @@
         <v>69</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>17</v>
@@ -1581,7 +1581,7 @@
         <v>76</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>19</v>
@@ -1601,7 +1601,7 @@
         <v>79</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>20</v>
@@ -1621,7 +1621,7 @@
         <v>81</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>20</v>
@@ -1641,7 +1641,7 @@
         <v>81</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>20</v>
@@ -1661,7 +1661,7 @@
         <v>81</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>20</v>
@@ -1741,7 +1741,7 @@
         <v>91</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>26</v>
@@ -1761,7 +1761,7 @@
         <v>91</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>26</v>
@@ -1793,7 +1793,7 @@
         <v>96</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>28</v>
@@ -1837,7 +1837,7 @@
         <v>101</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>31</v>
@@ -1857,7 +1857,7 @@
         <v>101</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>31</v>
@@ -1877,7 +1877,7 @@
         <v>101</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>31</v>
@@ -1897,7 +1897,7 @@
         <v>101</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>31</v>
@@ -1929,7 +1929,7 @@
         <v>108</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>33</v>
@@ -1949,7 +1949,7 @@
         <v>111</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>34</v>
@@ -1981,7 +1981,7 @@
         <v>115</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>36</v>
@@ -2025,7 +2025,7 @@
         <v>120</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E72" s="5" t="n">
         <v>39</v>
@@ -2045,7 +2045,7 @@
         <v>120</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E73" s="5" t="n">
         <v>39</v>
@@ -2113,7 +2113,7 @@
         <v>128</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E78" s="5" t="n">
         <v>44</v>
@@ -2133,7 +2133,7 @@
         <v>128</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E79" s="5" t="n">
         <v>44</v>
@@ -2153,7 +2153,7 @@
         <v>128</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E80" s="5" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
weekly forward look stats update 15.11.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 08 November 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 15 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,28 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">11 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 November 2024</t>
+    <t xml:space="preserve">18 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
@@ -896,7 +887,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -904,13 +895,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -924,13 +915,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -944,19 +935,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -964,16 +955,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>48</v>
@@ -984,19 +975,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -1013,10 +1004,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1033,10 +1024,10 @@
         <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1044,16 +1035,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>51</v>
@@ -1064,16 +1055,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>51</v>
@@ -1084,96 +1075,96 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>5</v>
@@ -1184,16 +1175,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>5</v>
@@ -1204,16 +1195,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>5</v>
@@ -1224,16 +1215,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>5</v>
@@ -1244,16 +1235,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>5</v>
@@ -1264,60 +1255,60 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>8</v>
@@ -1328,92 +1319,92 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13</v>
@@ -1424,72 +1415,72 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>17</v>
@@ -1500,16 +1491,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>17</v>
@@ -1520,16 +1511,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>17</v>
@@ -1540,35 +1531,35 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
@@ -1581,10 +1572,10 @@
         <v>76</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1592,16 +1583,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>20</v>
@@ -1612,16 +1603,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>20</v>
@@ -1632,16 +1623,16 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>20</v>
@@ -1652,96 +1643,96 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="D54" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="C55" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>26</v>
@@ -1752,92 +1743,92 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>31</v>
@@ -1848,16 +1839,16 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>31</v>
@@ -1868,16 +1859,16 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>31</v>
@@ -1888,35 +1879,35 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
@@ -1929,10 +1920,10 @@
         <v>108</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1942,90 +1933,90 @@
       <c r="A67" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="D68" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="C72" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E72" s="5" t="n">
         <v>39</v>
@@ -2036,84 +2027,84 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F76" s="5"/>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E77" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="C78" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E78" s="5" t="n">
         <v>44</v>
@@ -2124,16 +2115,16 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E79" s="5" t="n">
         <v>44</v>
@@ -2142,28 +2133,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E80" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F80">
+  <conditionalFormatting sqref="A5:F79">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2174,7 +2145,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A80">
+  <conditionalFormatting sqref="A5:A79">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 22.11.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 15 November 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 22 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">18 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: June 2024.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 November 2024</t>
+    <t xml:space="preserve">25 Nov 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,21 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 November 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2023 to 2024</t>
   </si>
   <si>
@@ -80,10 +65,13 @@
     <t xml:space="preserve">02 Dec 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Prison Population Projections: 2024 - 2029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Civil justice statistics: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">09 Dec 2024</t>
@@ -887,7 +875,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -904,10 +892,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -915,19 +903,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -938,7 +926,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -947,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -955,19 +943,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -975,19 +963,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -995,19 +983,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -1015,16 +1003,16 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>51</v>
@@ -1035,116 +1023,116 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>5</v>
@@ -1155,16 +1143,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>5</v>
@@ -1175,16 +1163,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>5</v>
@@ -1195,16 +1183,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>5</v>
@@ -1215,103 +1203,95 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1325,7 +1305,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F30" s="5"/>
     </row>
@@ -1333,134 +1313,142 @@
       <c r="A31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>17</v>
@@ -1471,16 +1459,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>17</v>
@@ -1491,39 +1479,31 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1533,29 +1513,37 @@
       <c r="A43" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="B43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="5" t="n">
         <v>20</v>
-      </c>
-      <c r="E44" s="5" t="n">
-        <v>19</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1563,16 +1551,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>20</v>
@@ -1583,16 +1571,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>20</v>
@@ -1603,139 +1591,131 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1749,7 +1729,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F56" s="5"/>
     </row>
@@ -1757,58 +1737,66 @@
       <c r="A57" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="C60" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>31</v>
@@ -1819,16 +1807,16 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>31</v>
@@ -1839,39 +1827,31 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1881,33 +1861,33 @@
       <c r="A64" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C65" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
@@ -1920,10 +1900,10 @@
         <v>108</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1937,7 +1917,7 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F67" s="5"/>
     </row>
@@ -1945,146 +1925,154 @@
       <c r="A68" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="D69" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F75" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F76" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="C77" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E77" s="5" t="n">
         <v>44</v>
@@ -2093,48 +2081,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E78" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E79" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F79">
+  <conditionalFormatting sqref="A5:F77">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2145,7 +2093,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A79">
+  <conditionalFormatting sqref="A5:A77">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 29.11.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 22 November 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 29 November 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">25 Nov 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service Staff Equalities Report: 2023 to 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 November 2024</t>
+    <t xml:space="preserve">02 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Population Projections: 2024 - 2029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,42 +56,36 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">HM Prison and Probation Service offender equalities report: 2023 to 2024</t>
+    <t xml:space="preserve">Civil justice statistics: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female Offender Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">02 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Population Projections: 2024 - 2029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 December 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
   </si>
   <si>
@@ -99,6 +93,15 @@
   </si>
   <si>
     <t xml:space="preserve">23 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Alcohol Monitoring Statistics Publication, Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad-hoc</t>
   </si>
   <si>
     <t xml:space="preserve">29 Dec 2025</t>
@@ -875,7 +878,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -892,10 +895,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -903,19 +906,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -923,19 +926,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -952,10 +955,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -963,16 +966,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>51</v>
@@ -983,16 +986,16 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>51</v>
@@ -1003,96 +1006,104 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>5</v>
@@ -1103,16 +1114,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>5</v>
@@ -1123,16 +1134,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>5</v>
@@ -1143,16 +1154,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>5</v>
@@ -1163,16 +1174,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>5</v>
@@ -1183,60 +1194,60 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>8</v>
@@ -1247,92 +1258,92 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13</v>
@@ -1343,72 +1354,72 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>17</v>
@@ -1419,16 +1430,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>17</v>
@@ -1439,16 +1450,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>17</v>
@@ -1459,51 +1470,51 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1511,16 +1522,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>20</v>
@@ -1531,16 +1542,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>20</v>
@@ -1551,16 +1562,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>20</v>
@@ -1571,96 +1582,96 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>26</v>
@@ -1671,92 +1682,92 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>31</v>
@@ -1767,16 +1778,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="D59" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>31</v>
@@ -1787,16 +1798,16 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>31</v>
@@ -1807,51 +1818,51 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1859,92 +1870,92 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>39</v>
@@ -1955,84 +1966,84 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E74" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F74" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>44</v>
@@ -2043,16 +2054,16 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E76" s="5" t="n">
         <v>44</v>
@@ -2061,28 +2072,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E77" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F77">
+  <conditionalFormatting sqref="A5:F76">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2093,7 +2084,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A77">
+  <conditionalFormatting sqref="A5:A76">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 06.12.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 29 November 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">02 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prison Population Projections: 2024 - 2029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 December 2024</t>
+    <t xml:space="preserve">09 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,18 +56,9 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Civil justice statistics: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Dec 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tribunals statistics quarterly: July to September 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">12 December 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Female Offender Dashboard</t>
   </si>
   <si>
@@ -83,48 +74,45 @@
     <t xml:space="preserve">19 December 2024</t>
   </si>
   <si>
+    <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ad-Hoc Alcohol Monitoring Statistics Publication, Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad-hoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 Dec 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 January 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Alcohol Monitoring Statistics Publication, Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Dec 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 January 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
   </si>
   <si>
@@ -134,6 +122,9 @@
     <t xml:space="preserve">Justice data lab statistics: January 2025.</t>
   </si>
   <si>
+    <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
   </si>
   <si>
@@ -387,6 +378,27 @@
   </si>
   <si>
     <t xml:space="preserve">Deaths of offenders supervised in the community, England and Wales, 2024/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 Dec 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Civil justice statistics: July to September 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 December 2025</t>
   </si>
 </sst>
 </file>
@@ -878,7 +890,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -898,7 +910,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -906,13 +918,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -926,7 +938,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -938,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -946,16 +958,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>51</v>
@@ -966,124 +978,124 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E16" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>5</v>
@@ -1094,16 +1106,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>5</v>
@@ -1114,16 +1126,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>5</v>
@@ -1134,16 +1146,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>5</v>
@@ -1154,16 +1166,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>5</v>
@@ -1174,60 +1186,60 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>8</v>
@@ -1238,92 +1250,92 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13</v>
@@ -1334,72 +1346,72 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>17</v>
@@ -1410,16 +1422,16 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>17</v>
@@ -1430,16 +1442,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>17</v>
@@ -1450,35 +1462,35 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
@@ -1491,10 +1503,10 @@
         <v>70</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1502,16 +1514,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>20</v>
@@ -1522,16 +1534,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>20</v>
@@ -1542,16 +1554,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>20</v>
@@ -1562,96 +1574,96 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>26</v>
@@ -1662,92 +1674,92 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="D53" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>31</v>
@@ -1758,16 +1770,16 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>31</v>
@@ -1778,16 +1790,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>31</v>
@@ -1798,35 +1810,35 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
@@ -1839,10 +1851,10 @@
         <v>102</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1852,90 +1864,90 @@
       <c r="A63" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="C68" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>39</v>
@@ -1946,84 +1958,84 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F70" s="5"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E73" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F73" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="C74" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E74" s="5" t="n">
         <v>44</v>
@@ -2034,16 +2046,16 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>44</v>
@@ -2054,26 +2066,74 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E76" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F76" s="5" t="s">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E80" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="F80" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F76">
+  <conditionalFormatting sqref="A5:F80">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2084,7 +2144,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A76">
+  <conditionalFormatting sqref="A5:A80">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 13.12.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 December 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -44,10 +44,10 @@
     <t xml:space="preserve">09 Dec 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 December 2024</t>
+    <t xml:space="preserve">Female Offender Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,15 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female Offender Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 December 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">16 Dec 2024</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
   </si>
   <si>
-    <t xml:space="preserve">Justice data lab statistics: January 2025.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
   </si>
   <si>
@@ -137,6 +125,12 @@
     <t xml:space="preserve">10 Feb 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Mortgage and landlord possession statistics: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 February 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">17 Feb 2025</t>
   </si>
   <si>
@@ -164,6 +158,12 @@
     <t xml:space="preserve">10 Mar 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 March 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">17 Mar 2025</t>
   </si>
   <si>
@@ -221,12 +221,6 @@
     <t xml:space="preserve">12 May 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 May 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2025.</t>
   </si>
   <si>
@@ -248,7 +242,19 @@
     <t xml:space="preserve">02 Jun 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Civil justice statistics: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 June 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">09 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">16 Jun 2025</t>
@@ -898,19 +904,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -918,10 +924,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -930,7 +936,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -938,124 +944,124 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>5</v>
@@ -1066,16 +1072,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>5</v>
@@ -1086,16 +1092,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>5</v>
@@ -1106,16 +1112,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>5</v>
@@ -1126,39 +1132,31 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1166,19 +1164,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1188,41 +1186,49 @@
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E22" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1230,19 +1236,19 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1250,31 +1256,31 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1282,116 +1288,132 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>17</v>
@@ -1402,39 +1424,31 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1442,19 +1456,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1462,31 +1476,39 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1494,59 +1516,43 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1554,19 +1560,19 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1574,131 +1580,147 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1706,63 +1728,71 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="E56" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1770,19 +1800,19 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
@@ -1790,103 +1820,95 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1894,246 +1916,182 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E70" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E71" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
       <c r="E75" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F75" s="5"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+        <v>128</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E76" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F78" s="5"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F76" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F80">
+  <conditionalFormatting sqref="A5:F76">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2144,7 +2102,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A80">
+  <conditionalFormatting sqref="A5:A76">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 19.12.24
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 December 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 19 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">09 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female Offender Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 December 2024</t>
+    <t xml:space="preserve">16 Dec 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,15 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">16 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 December 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
   </si>
   <si>
@@ -101,13 +92,13 @@
     <t xml:space="preserve">30 January 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
   </si>
   <si>
     <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
@@ -896,7 +887,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -904,13 +895,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -924,104 +915,104 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8" t="n">
-        <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>5</v>
@@ -1032,16 +1023,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>5</v>
@@ -1052,16 +1043,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>5</v>
@@ -1072,16 +1063,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>5</v>
@@ -1092,16 +1083,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>5</v>
@@ -1112,35 +1103,35 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
@@ -1153,10 +1144,10 @@
         <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1164,16 +1155,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>8</v>
@@ -1184,35 +1175,35 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
@@ -1225,10 +1216,10 @@
         <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1238,46 +1229,46 @@
       <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13</v>
@@ -1288,72 +1279,72 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>17</v>
@@ -1364,16 +1355,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>17</v>
@@ -1384,16 +1375,16 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>17</v>
@@ -1404,35 +1395,35 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
@@ -1445,10 +1436,10 @@
         <v>67</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1456,16 +1447,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>20</v>
@@ -1476,16 +1467,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>20</v>
@@ -1496,47 +1487,47 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
@@ -1549,10 +1540,10 @@
         <v>77</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1562,46 +1553,46 @@
       <c r="A44" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>26</v>
@@ -1612,92 +1603,92 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="E49" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C52" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>31</v>
@@ -1708,16 +1699,16 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>31</v>
@@ -1728,16 +1719,16 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>31</v>
@@ -1748,35 +1739,35 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
@@ -1789,10 +1780,10 @@
         <v>101</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1802,90 +1793,90 @@
       <c r="A58" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="C63" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>39</v>
@@ -1896,84 +1887,84 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="D68" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="C69" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>44</v>
@@ -1984,16 +1975,16 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>44</v>
@@ -2004,94 +1995,74 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F72" s="5"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F73" s="5"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F74" s="5"/>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E75" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E76" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F75" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F76">
+  <conditionalFormatting sqref="A5:F75">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2102,7 +2073,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A76">
+  <conditionalFormatting sqref="A5:A75">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 03.01.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 19 December 2024</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 03 January 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">16 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 December 2024</t>
+    <t xml:space="preserve">27 Jan 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 January 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,55 +56,19 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve"> Legal aid statistics quarterly: July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad-Hoc Alcohol Monitoring Statistics Publication, Dec 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad-hoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 Dec 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 January 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
   </si>
   <si>
+    <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
   </si>
   <si>
     <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
@@ -887,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -907,7 +871,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -915,87 +879,111 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8"/>
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1003,19 +991,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1023,19 +1011,19 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
@@ -1043,39 +1031,31 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1083,19 +1063,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1103,31 +1083,31 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1138,16 +1118,16 @@
         <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1155,71 +1135,55 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1227,31 +1191,39 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1259,19 +1231,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1279,55 +1251,71 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1335,19 +1323,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1355,71 +1343,63 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
@@ -1427,39 +1407,31 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1467,19 +1439,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1487,95 +1459,95 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1583,19 +1555,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1603,95 +1575,103 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1699,71 +1679,63 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1771,95 +1743,87 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1867,19 +1831,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="C63" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1887,182 +1851,74 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E69" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E70" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F72" s="5"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E75" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F75">
+  <conditionalFormatting sqref="A5:F68">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2073,7 +1929,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A75">
+  <conditionalFormatting sqref="A5:A68">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look update 10.01.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 03 January 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 10 January 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -86,15 +86,21 @@
     <t xml:space="preserve">13 February 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Coroners statistics 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">17 Feb 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 February 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">20 February 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
   </si>
   <si>
@@ -165,9 +171,6 @@
   </si>
   <si>
     <t xml:space="preserve">05 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroners statistics 2024</t>
   </si>
   <si>
     <t xml:space="preserve">8 May 2025</t>
@@ -991,19 +994,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1011,13 +1014,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>18</v>
@@ -1031,31 +1034,39 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1063,51 +1074,51 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1115,47 +1126,55 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E22" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
@@ -1165,7 +1184,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F23" s="5"/>
     </row>
@@ -1173,51 +1192,35 @@
       <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>18</v>
@@ -1231,13 +1234,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>18</v>
@@ -1251,31 +1254,39 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1283,39 +1294,31 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="D31" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1323,13 +1326,13 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>18</v>
@@ -1343,95 +1346,103 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1441,49 +1452,49 @@
       <c r="A39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1491,77 +1502,69 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>18</v>
@@ -1575,13 +1578,13 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>18</v>
@@ -1595,31 +1598,39 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1627,51 +1638,51 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1679,165 +1690,157 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>18</v>
@@ -1851,74 +1854,114 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="B70" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="5" t="n">
+      <c r="C70" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F70" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F68">
+  <conditionalFormatting sqref="A5:F70">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1929,7 +1972,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A68">
+  <conditionalFormatting sqref="A5:A70">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look stats weekly update 17.01.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 10 January 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 17 January 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -191,6 +191,9 @@
     <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">19 May 2025</t>
   </si>
   <si>
@@ -281,12 +284,15 @@
     <t xml:space="preserve">18 Aug 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 August 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: June 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">21 August 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">25 Aug 2025</t>
   </si>
   <si>
@@ -302,6 +308,12 @@
     <t xml:space="preserve">08 Sep 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: April to June 2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 September 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">15 Sep 2025</t>
   </si>
   <si>
@@ -353,9 +365,24 @@
     <t xml:space="preserve">17 Nov 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  April to June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 November 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HM Prison and Probation Service workforce quarterly: September 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 Nov 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Her Majesty’s Prison and Probation Service offender equalities report: 2024 to 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 November 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">01 Dec 2025</t>
   </si>
   <si>
@@ -363,6 +390,27 @@
   </si>
   <si>
     <t xml:space="preserve">4 December 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 Dec 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: July to September 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 December 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Dec 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: July to September 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 December 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: July to September 2025</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1111,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>8</v>
@@ -1386,15 +1434,23 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
@@ -1404,7 +1460,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -1412,37 +1468,29 @@
       <c r="A37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1450,45 +1498,45 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>18</v>
@@ -1502,47 +1550,55 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
@@ -1552,7 +1608,7 @@
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F45" s="5"/>
     </row>
@@ -1560,31 +1616,23 @@
       <c r="A46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>18</v>
@@ -1598,13 +1646,13 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>18</v>
@@ -1618,13 +1666,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>18</v>
@@ -1638,51 +1686,51 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="D52" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1690,31 +1738,39 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="D53" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1722,27 +1778,35 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
@@ -1758,7 +1822,7 @@
         <v>18</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1766,121 +1830,113 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="B59" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B64" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>18</v>
@@ -1894,74 +1950,210 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E66" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="E67" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F69" s="5"/>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C70" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="5" t="n">
+      <c r="B71" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F73" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F70">
+  <conditionalFormatting sqref="A5:F76">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1972,7 +2164,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A70">
+  <conditionalFormatting sqref="A5:A76">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 24.01.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 17 January 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 24 January 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -68,12 +68,12 @@
     <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
   </si>
   <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">03 Feb 2025</t>
   </si>
   <si>
@@ -92,19 +92,22 @@
     <t xml:space="preserve">17 Feb 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 February 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">20 February 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Feb 2025</t>
+    <t xml:space="preserve">27 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">03 Mar 2025</t>
@@ -131,12 +134,15 @@
     <t xml:space="preserve">24 Mar 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 March 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
   </si>
   <si>
-    <t xml:space="preserve">27 March 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
   </si>
   <si>
@@ -404,10 +410,13 @@
     <t xml:space="preserve">15 Dec 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Family court statistics quarterly: July to September 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 December 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Criminal court statistics quarterly: July to September 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 December 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Legal aid statistics quarterly: July to September 2025</t>
@@ -979,7 +988,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>5</v>
@@ -993,13 +1002,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>5</v>
@@ -1051,7 +1060,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>7</v>
@@ -1071,7 +1080,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>8</v>
@@ -1102,19 +1111,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1122,31 +1131,39 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1154,48 +1171,48 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E19" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13</v>
@@ -1206,16 +1223,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13</v>
@@ -1226,7 +1243,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1238,7 +1255,7 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1250,7 +1267,7 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1262,16 +1279,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>17</v>
@@ -1282,16 +1299,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>17</v>
@@ -1302,16 +1319,16 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>17</v>
@@ -1322,16 +1339,16 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>17</v>
@@ -1342,7 +1359,7 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1354,16 +1371,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>19</v>
@@ -1374,16 +1391,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>20</v>
@@ -1394,16 +1411,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>20</v>
@@ -1414,16 +1431,16 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>20</v>
@@ -1434,16 +1451,16 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>20</v>
@@ -1454,7 +1471,7 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1466,7 +1483,7 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1478,13 +1495,13 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>12</v>
@@ -1498,13 +1515,13 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>12</v>
@@ -1518,7 +1535,7 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1530,16 +1547,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>26</v>
@@ -1550,16 +1567,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>26</v>
@@ -1570,7 +1587,7 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1582,16 +1599,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>28</v>
@@ -1602,7 +1619,7 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1614,7 +1631,7 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1626,16 +1643,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>31</v>
@@ -1646,16 +1663,16 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>31</v>
@@ -1666,16 +1683,16 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>31</v>
@@ -1686,16 +1703,16 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>31</v>
@@ -1706,7 +1723,7 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1718,16 +1735,16 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>33</v>
@@ -1738,16 +1755,16 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>34</v>
@@ -1758,16 +1775,16 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>34</v>
@@ -1778,7 +1795,7 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1790,16 +1807,16 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>36</v>
@@ -1810,16 +1827,16 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>37</v>
@@ -1830,7 +1847,7 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -1842,16 +1859,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>39</v>
@@ -1862,16 +1879,16 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>39</v>
@@ -1882,7 +1899,7 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -1894,7 +1911,7 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -1906,7 +1923,7 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -1918,7 +1935,7 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -1930,16 +1947,16 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E65" s="5" t="n">
         <v>44</v>
@@ -1950,16 +1967,16 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E66" s="5" t="n">
         <v>44</v>
@@ -1970,16 +1987,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="D67" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>44</v>
@@ -1990,7 +2007,7 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -2002,7 +2019,7 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -2014,16 +2031,16 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>47</v>
@@ -2034,16 +2051,16 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E71" s="5" t="n">
         <v>47</v>
@@ -2054,16 +2071,16 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E72" s="5" t="n">
         <v>48</v>
@@ -2074,16 +2091,16 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E73" s="5" t="n">
         <v>49</v>
@@ -2094,16 +2111,16 @@
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E74" s="5" t="n">
         <v>50</v>
@@ -2114,16 +2131,16 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E75" s="5" t="n">
         <v>51</v>
@@ -2134,16 +2151,16 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E76" s="5" t="n">
         <v>51</v>
@@ -2152,8 +2169,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F76">
+  <conditionalFormatting sqref="A5:F77">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2164,7 +2201,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A76">
+  <conditionalFormatting sqref="A5:A77">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 13.02.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 24 January 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">27 Jan 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youth Justice Statistics: 2023 - 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 January 2025</t>
+    <t xml:space="preserve">17 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,129 +56,102 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: July to September 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women and the Criminal Justice System 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: January 2023 to March 2023 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to September 2024</t>
+    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 February 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">03 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 February 2025</t>
+    <t xml:space="preserve">10 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 April 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: April to June 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offender management statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Coroners statistics 2024</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 February 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 February 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 April 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 May 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">8 May 2025</t>
   </si>
   <si>
@@ -267,6 +240,9 @@
   </si>
   <si>
     <t xml:space="preserve">Offender management statistics quarterly: January 2025 to March 2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proven reoffending statistics: July 2023 and September 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
@@ -911,7 +887,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -931,7 +907,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -939,19 +915,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -959,19 +935,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -979,19 +955,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -999,19 +975,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -1019,31 +995,39 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1051,19 +1035,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -1071,79 +1055,55 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1151,19 +1111,19 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1171,31 +1131,39 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1203,19 +1171,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1223,19 +1191,19 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1243,55 +1211,71 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1302,16 +1286,16 @@
         <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1322,16 +1306,16 @@
         <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1342,16 +1326,16 @@
         <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1359,71 +1343,63 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1431,19 +1407,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1451,67 +1427,67 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
@@ -1524,10 +1500,10 @@
         <v>69</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1541,7 +1517,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F40" s="5"/>
     </row>
@@ -1549,37 +1525,29 @@
       <c r="A41" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1587,31 +1555,39 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="C44" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1619,63 +1595,71 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="C48" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1683,19 +1667,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1703,19 +1687,19 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1729,7 +1713,7 @@
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F51" s="5"/>
     </row>
@@ -1744,10 +1728,10 @@
         <v>90</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
@@ -1764,10 +1748,10 @@
         <v>93</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1775,51 +1759,51 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="B55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1829,157 +1813,149 @@
       <c r="A57" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F64" s="5"/>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="C66" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1987,19 +1963,19 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -2007,43 +1983,59 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="D68" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="B69" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>13</v>
@@ -2051,19 +2043,19 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E71" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>13</v>
@@ -2071,19 +2063,19 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E72" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>13</v>
@@ -2091,106 +2083,26 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="D73" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E73" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E76" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F77">
+  <conditionalFormatting sqref="A5:F73">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2201,7 +2113,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A77">
+  <conditionalFormatting sqref="A5:A73">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 21.02.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 February 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,31 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 February 2025</t>
+    <t xml:space="preserve">24 Feb 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  July to September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">03 Mar 2025</t>
@@ -887,7 +875,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -895,19 +883,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -915,19 +903,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -935,19 +923,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -955,19 +943,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -975,19 +963,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -995,16 +983,16 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>13</v>
@@ -1015,92 +1003,92 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
@@ -1111,16 +1099,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>17</v>
@@ -1131,16 +1119,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>17</v>
@@ -1151,16 +1139,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>17</v>
@@ -1171,39 +1159,31 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1213,29 +1193,37 @@
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1243,16 +1231,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>20</v>
@@ -1263,16 +1251,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>20</v>
@@ -1283,16 +1271,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>20</v>
@@ -1303,16 +1291,16 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>20</v>
@@ -1323,87 +1311,79 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
@@ -1416,10 +1396,10 @@
         <v>60</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1427,51 +1407,51 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1485,7 +1465,7 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F38" s="5"/>
     </row>
@@ -1493,58 +1473,66 @@
       <c r="A39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="C42" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>31</v>
@@ -1555,16 +1543,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>31</v>
@@ -1575,16 +1563,16 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>31</v>
@@ -1595,39 +1583,31 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1637,29 +1617,37 @@
       <c r="A47" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="B47" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1669,37 +1657,29 @@
       <c r="A49" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1709,33 +1689,33 @@
       <c r="A51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="B51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
@@ -1748,10 +1728,10 @@
         <v>93</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1759,116 +1739,124 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>44</v>
@@ -1879,67 +1867,67 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F63" s="5"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E64" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E65" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
@@ -1952,10 +1940,10 @@
         <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1963,19 +1951,19 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -1983,19 +1971,19 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>13</v>
@@ -2003,19 +1991,19 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E69" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>13</v>
@@ -2023,19 +2011,19 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="D70" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>13</v>
@@ -2043,16 +2031,16 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="C71" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E71" s="5" t="n">
         <v>51</v>
@@ -2061,48 +2049,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E72" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E73" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F73">
+  <conditionalFormatting sqref="A5:F71">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2113,7 +2061,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A73">
+  <conditionalFormatting sqref="A5:A71">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 28.02.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 February 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 February 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,40 +41,31 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">24 Feb 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: September 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 February 2025</t>
+    <t xml:space="preserve">03 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">17 Mar 2025</t>
@@ -875,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -895,7 +886,7 @@
         <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -912,10 +903,10 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -935,7 +926,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -943,16 +934,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>13</v>
@@ -963,13 +954,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -983,72 +974,72 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>17</v>
@@ -1059,13 +1050,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1079,16 +1070,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
@@ -1099,16 +1090,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>17</v>
@@ -1119,16 +1110,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>17</v>
@@ -1139,35 +1130,35 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
@@ -1183,7 +1174,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1191,13 +1182,13 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
@@ -1211,16 +1202,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>20</v>
@@ -1231,16 +1222,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>20</v>
@@ -1251,13 +1242,13 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>17</v>
@@ -1271,16 +1262,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>20</v>
@@ -1291,47 +1282,47 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
@@ -1344,10 +1335,10 @@
         <v>53</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1357,46 +1348,46 @@
       <c r="A32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C34" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>26</v>
@@ -1407,92 +1398,92 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>31</v>
@@ -1503,16 +1494,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>31</v>
@@ -1523,16 +1514,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>31</v>
@@ -1543,16 +1534,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>31</v>
@@ -1563,35 +1554,35 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
@@ -1604,10 +1595,10 @@
         <v>78</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1615,16 +1606,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>34</v>
@@ -1635,35 +1626,35 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
@@ -1676,10 +1667,10 @@
         <v>86</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
@@ -1689,46 +1680,46 @@
       <c r="A51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="C53" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>39</v>
@@ -1739,84 +1730,84 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>44</v>
@@ -1827,16 +1818,16 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>44</v>
@@ -1847,60 +1838,60 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F62" s="5"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E63" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="C64" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E64" s="5" t="n">
         <v>47</v>
@@ -1911,19 +1902,19 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="D65" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>13</v>
@@ -1940,10 +1931,10 @@
         <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1960,10 +1951,10 @@
         <v>115</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -1980,10 +1971,10 @@
         <v>118</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E68" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>13</v>
@@ -1991,16 +1982,16 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="C69" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>51</v>
@@ -2011,16 +2002,16 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E70" s="5" t="n">
         <v>51</v>
@@ -2029,28 +2020,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E71" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F71">
+  <conditionalFormatting sqref="A5:F70">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2061,7 +2032,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A71">
+  <conditionalFormatting sqref="A5:A70">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
stats forward look weekly update 07.03.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 February 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 07 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,49 +41,40 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">03 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil Justice Statistics: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 March 2025</t>
+    <t xml:space="preserve">10 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
@@ -866,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -883,10 +874,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -894,19 +885,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -914,16 +905,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E8" t="n">
         <v>13</v>
@@ -934,13 +925,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
@@ -954,72 +945,72 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>17</v>
@@ -1030,16 +1021,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>17</v>
@@ -1050,16 +1041,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>17</v>
@@ -1070,16 +1061,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
@@ -1090,16 +1081,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>17</v>
@@ -1110,35 +1101,35 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
@@ -1154,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1162,16 +1153,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>20</v>
@@ -1182,16 +1173,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>20</v>
@@ -1202,16 +1193,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>20</v>
@@ -1222,13 +1213,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>12</v>
@@ -1242,16 +1233,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>20</v>
@@ -1262,47 +1253,47 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
@@ -1315,10 +1306,10 @@
         <v>50</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1328,46 +1319,46 @@
       <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>26</v>
@@ -1378,92 +1369,92 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C39" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>31</v>
@@ -1474,16 +1465,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>31</v>
@@ -1494,16 +1485,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>31</v>
@@ -1514,16 +1505,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>31</v>
@@ -1534,35 +1525,35 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
@@ -1575,10 +1566,10 @@
         <v>75</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1586,16 +1577,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>34</v>
@@ -1606,35 +1597,35 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
@@ -1647,10 +1638,10 @@
         <v>83</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1660,46 +1651,46 @@
       <c r="A50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="C52" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>39</v>
@@ -1710,84 +1701,84 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>44</v>
@@ -1798,16 +1789,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>44</v>
@@ -1818,60 +1809,60 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E62" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="C63" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E63" s="5" t="n">
         <v>47</v>
@@ -1882,19 +1873,19 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1911,10 +1902,10 @@
         <v>109</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>13</v>
@@ -1931,10 +1922,10 @@
         <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1951,10 +1942,10 @@
         <v>115</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>13</v>
@@ -1962,16 +1953,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C68" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>51</v>
@@ -1982,16 +1973,16 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E69" s="5" t="n">
         <v>51</v>
@@ -2000,28 +1991,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F70">
+  <conditionalFormatting sqref="A5:F69">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2032,7 +2003,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A70">
+  <conditionalFormatting sqref="A5:A69">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 14.03.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 07 March 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,28 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 March 2025</t>
+    <t xml:space="preserve">17 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">24 Mar 2025</t>
@@ -857,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -874,10 +865,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -885,16 +876,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="n">
         <v>13</v>
@@ -905,16 +896,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
         <v>13</v>
@@ -925,69 +916,69 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -1001,16 +992,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>17</v>
@@ -1021,16 +1012,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>17</v>
@@ -1041,16 +1032,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>17</v>
@@ -1061,16 +1052,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>17</v>
@@ -1081,35 +1072,35 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E19" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
@@ -1122,10 +1113,10 @@
         <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <v>20</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1133,16 +1124,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>20</v>
@@ -1153,16 +1144,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>20</v>
@@ -1173,16 +1164,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>20</v>
@@ -1193,16 +1184,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>20</v>
@@ -1213,13 +1204,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>12</v>
@@ -1233,47 +1224,47 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
@@ -1289,7 +1280,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1299,46 +1290,46 @@
       <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>26</v>
@@ -1349,92 +1340,92 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>31</v>
@@ -1445,16 +1436,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>31</v>
@@ -1465,16 +1456,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>31</v>
@@ -1485,16 +1476,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>31</v>
@@ -1505,35 +1496,35 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
@@ -1546,10 +1537,10 @@
         <v>72</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1557,16 +1548,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C45" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>34</v>
@@ -1577,35 +1568,35 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
@@ -1618,10 +1609,10 @@
         <v>80</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1631,46 +1622,46 @@
       <c r="A49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>39</v>
@@ -1681,84 +1672,84 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="C57" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>44</v>
@@ -1769,16 +1760,16 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>44</v>
@@ -1789,60 +1780,60 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="C62" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>47</v>
@@ -1853,19 +1844,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1882,10 +1873,10 @@
         <v>106</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1902,10 +1893,10 @@
         <v>109</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>13</v>
@@ -1922,10 +1913,10 @@
         <v>112</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1933,16 +1924,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="C67" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>51</v>
@@ -1953,16 +1944,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>51</v>
@@ -1971,28 +1962,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E69" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F69">
+  <conditionalFormatting sqref="A5:F68">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2003,7 +1974,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A69">
+  <conditionalFormatting sqref="A5:A68">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look stats weekly update 21.03.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 14 March 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,42 +41,39 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Profile of Repeat Offending by Children and Young People in England and Wales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 March 2025</t>
+    <t xml:space="preserve">24 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">31 Mar 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Trainee Probation Officer recruitment: April 2024 to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 April 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">07 Apr 2025</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
     <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal justice statistics quarterly: December 2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2024</t>
   </si>
   <si>
@@ -164,10 +164,13 @@
     <t xml:space="preserve">23 Jun 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 June 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
@@ -848,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -856,16 +859,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
         <v>13</v>
@@ -876,16 +879,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="E7" t="n">
         <v>13</v>
@@ -896,19 +899,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="n">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="n">
-        <v>13</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -922,7 +925,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -934,7 +937,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -942,26 +945,34 @@
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>17</v>
@@ -972,13 +983,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -992,16 +1003,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>17</v>
@@ -1012,16 +1023,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>17</v>
@@ -1032,16 +1043,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>17</v>
@@ -1052,51 +1063,51 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1104,13 +1115,13 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
@@ -1124,16 +1135,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>20</v>
@@ -1144,16 +1155,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>20</v>
@@ -1164,16 +1175,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>20</v>
@@ -1184,16 +1195,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>20</v>
@@ -1204,16 +1215,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>20</v>
@@ -1257,7 +1268,7 @@
         <v>44</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>23</v>
@@ -1277,7 +1288,7 @@
         <v>47</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>24</v>
@@ -1309,7 +1320,7 @@
         <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>26</v>
@@ -1329,7 +1340,7 @@
         <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>26</v>
@@ -1340,47 +1351,55 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
@@ -1390,7 +1409,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -1398,34 +1417,26 @@
       <c r="A37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>31</v>
@@ -1436,16 +1447,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>31</v>
@@ -1456,16 +1467,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>31</v>
@@ -1476,16 +1487,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>31</v>
@@ -1496,51 +1507,51 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1548,16 +1559,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>34</v>
@@ -1568,51 +1579,51 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1620,48 +1631,48 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>39</v>
@@ -1672,15 +1683,23 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
@@ -1690,7 +1709,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -1702,7 +1721,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F54" s="5"/>
     </row>
@@ -1714,7 +1733,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F55" s="5"/>
     </row>
@@ -1722,34 +1741,26 @@
       <c r="A56" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D57" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>44</v>
@@ -1760,16 +1771,16 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>44</v>
@@ -1780,15 +1791,23 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E59" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
@@ -1798,7 +1817,7 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -1806,34 +1825,26 @@
       <c r="A61" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="D62" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E62" s="5" t="n">
         <v>47</v>
@@ -1844,19 +1855,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="C63" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1864,19 +1875,19 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1884,19 +1895,19 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="D65" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>13</v>
@@ -1904,19 +1915,19 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="D66" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
@@ -1924,16 +1935,16 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="D67" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E67" s="5" t="n">
         <v>51</v>
@@ -1944,16 +1955,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E68" s="5" t="n">
         <v>51</v>
@@ -1962,8 +1973,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F68">
+  <conditionalFormatting sqref="A5:F69">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1974,7 +2005,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A68">
+  <conditionalFormatting sqref="A5:A69">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward looks stats weekly update 28.03.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 21 March 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,58 +41,43 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">24 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 March 2025</t>
+    <t xml:space="preserve">31 Mar 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainee Probation Officer recruitment: April 2024 to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 April 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 April 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: October to December 2024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trainee Probation Officer recruitment: April 2024 to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 April 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 April 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Proven reoffending statistics: April to June 2023</t>
@@ -851,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -859,59 +844,43 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7" t="n">
         <v>16</v>
       </c>
-      <c r="E7" t="n">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -919,40 +888,56 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>17</v>
@@ -963,16 +948,16 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>17</v>
@@ -983,16 +968,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>17</v>
@@ -1003,39 +988,31 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1043,19 +1020,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1063,31 +1040,39 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>13</v>
@@ -1095,16 +1080,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>20</v>
@@ -1115,16 +1100,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>20</v>
@@ -1135,13 +1120,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>12</v>
@@ -1155,13 +1140,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
@@ -1175,59 +1160,43 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1237,41 +1206,49 @@
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1279,19 +1256,19 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1299,51 +1276,51 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1351,23 +1328,15 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
@@ -1377,7 +1346,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F34" s="5"/>
     </row>
@@ -1392,10 +1361,10 @@
         <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1403,40 +1372,56 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>31</v>
@@ -1447,16 +1432,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>31</v>
@@ -1467,39 +1452,31 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1507,19 +1484,19 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1527,35 +1504,35 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
@@ -1568,10 +1545,10 @@
         <v>73</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1579,19 +1556,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1599,31 +1576,31 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1631,19 +1608,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1657,7 +1634,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1665,145 +1642,137 @@
       <c r="A51" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="D54" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F58" s="5"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="D59" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>13</v>
@@ -1811,43 +1780,59 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E60" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E61" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1855,19 +1840,19 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
@@ -1875,19 +1860,19 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>13</v>
@@ -1895,19 +1880,19 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>13</v>
@@ -1915,86 +1900,26 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="D66" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F69">
+  <conditionalFormatting sqref="A5:F66">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -2005,7 +1930,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A69">
+  <conditionalFormatting sqref="A5:A66">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward looks stats weekly update 04.04.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 28 March 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 04 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,34 +41,19 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">31 Mar 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trainee Probation Officer recruitment: April 2024 to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 April 2025</t>
+    <t xml:space="preserve">21 Apr 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
@@ -836,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -844,40 +829,56 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6"/>
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" t="n">
-        <v>16</v>
-      </c>
-      <c r="F7"/>
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
         <v>17</v>
@@ -888,16 +889,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>17</v>
@@ -908,16 +909,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>17</v>
@@ -928,39 +929,31 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -968,19 +961,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -988,31 +981,39 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -1020,16 +1021,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>20</v>
@@ -1040,16 +1041,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>20</v>
@@ -1060,16 +1061,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>20</v>
@@ -1080,16 +1081,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>20</v>
@@ -1100,59 +1101,43 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="E20" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>13</v>
@@ -1162,41 +1147,49 @@
       <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E23" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>13</v>
@@ -1204,19 +1197,19 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1224,51 +1217,51 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E27" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1276,23 +1269,15 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
@@ -1302,7 +1287,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -1317,10 +1302,10 @@
         <v>52</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1328,40 +1313,56 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>31</v>
@@ -1372,16 +1373,16 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>31</v>
@@ -1392,39 +1393,31 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1432,19 +1425,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1452,35 +1445,35 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
@@ -1493,10 +1486,10 @@
         <v>68</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1504,19 +1497,19 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1524,31 +1517,31 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1556,19 +1549,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1582,7 +1575,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -1590,145 +1583,137 @@
       <c r="A48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E53" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F55" s="5"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1736,43 +1721,59 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="B58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E58" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>13</v>
@@ -1780,19 +1781,19 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>13</v>
@@ -1800,19 +1801,19 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -1820,19 +1821,19 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1840,86 +1841,26 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F66">
+  <conditionalFormatting sqref="A5:F63">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1930,7 +1871,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A66">
+  <conditionalFormatting sqref="A5:A63">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look weekly stats update 11.04.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 04 April 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 11 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -77,10 +77,13 @@
     <t xml:space="preserve">05 May 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Unpaid Work Management Information, update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 May 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coroners statistics 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">12 May 2025</t>
@@ -878,7 +881,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
         <v>17</v>
@@ -918,7 +921,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>17</v>
@@ -961,19 +964,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -981,16 +984,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>20</v>
@@ -1001,13 +1004,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
@@ -1021,13 +1024,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>16</v>
@@ -1041,13 +1044,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>16</v>
@@ -1061,16 +1064,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>20</v>
@@ -1081,13 +1084,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>12</v>
@@ -1101,15 +1104,23 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E20" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
@@ -1119,7 +1130,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="5"/>
     </row>
@@ -1127,37 +1138,29 @@
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1165,45 +1168,45 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>16</v>
@@ -1217,13 +1220,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>16</v>
@@ -1237,47 +1240,55 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
@@ -1287,7 +1298,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -1295,31 +1306,23 @@
       <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>16</v>
@@ -1333,13 +1336,13 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>16</v>
@@ -1353,13 +1356,13 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>16</v>
@@ -1373,13 +1376,13 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>16</v>
@@ -1393,51 +1396,51 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D39" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1445,13 +1448,13 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>16</v>
@@ -1465,51 +1468,51 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="D43" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1517,45 +1520,45 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>16</v>
@@ -1569,15 +1572,23 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
@@ -1587,7 +1598,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -1599,7 +1610,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1611,7 +1622,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1619,31 +1630,23 @@
       <c r="A51" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>16</v>
@@ -1657,13 +1660,13 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>16</v>
@@ -1677,15 +1680,23 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
@@ -1695,7 +1706,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F55" s="5"/>
     </row>
@@ -1703,31 +1714,23 @@
       <c r="A56" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F56" s="5"/>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>16</v>
@@ -1741,19 +1744,19 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
@@ -1761,19 +1764,19 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="D59" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>13</v>
@@ -1781,19 +1784,19 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="D60" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>13</v>
@@ -1801,19 +1804,19 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="D61" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -1821,13 +1824,13 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>16</v>
@@ -1841,13 +1844,13 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>16</v>
@@ -1859,8 +1862,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F63">
+  <conditionalFormatting sqref="A5:F64">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1871,7 +1894,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A63">
+  <conditionalFormatting sqref="A5:A64">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 17.04.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 11 April 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 17 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMPPS Annual Digest, April 2024 to March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Prison Performance Ratings: 2024 to 2025</t>
@@ -1416,51 +1419,51 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="D40" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1468,13 +1471,13 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>16</v>
@@ -1488,51 +1491,51 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="D44" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1540,45 +1543,45 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>16</v>
@@ -1592,15 +1595,23 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
@@ -1610,7 +1621,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1622,7 +1633,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1634,7 +1645,7 @@
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" s="5"/>
     </row>
@@ -1642,31 +1653,23 @@
       <c r="A52" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>16</v>
@@ -1680,13 +1683,13 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>16</v>
@@ -1700,15 +1703,23 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E55" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
@@ -1718,7 +1729,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F56" s="5"/>
     </row>
@@ -1726,31 +1737,23 @@
       <c r="A57" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F57" s="5"/>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B58" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>16</v>
@@ -1764,19 +1767,19 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>13</v>
@@ -1784,19 +1787,19 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="D60" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>13</v>
@@ -1804,19 +1807,19 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="D61" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>13</v>
@@ -1824,19 +1827,19 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="D62" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>13</v>
@@ -1844,13 +1847,13 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>16</v>
@@ -1864,13 +1867,13 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>16</v>
@@ -1882,8 +1885,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F64">
+  <conditionalFormatting sqref="A5:F65">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1894,7 +1917,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A64">
+  <conditionalFormatting sqref="A5:A65">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
forward look weekly stats update 25.04.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 17 April 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 25 April 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,58 +41,34 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">21 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in the children and young people secure estate: Update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 April 2025</t>
+    <t xml:space="preserve">05 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unpaid Work Management Information, update to December 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroners statistics 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: April 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proven reoffending statistics: April to June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offender management statistics quarterly: October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Apr 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unpaid Work Management Information, update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroners statistics 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2025.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Mortgage and landlord possession statistics: January to March 2025</t>
@@ -827,7 +803,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -847,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -855,19 +831,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -875,19 +851,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -895,19 +871,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -915,19 +891,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -935,31 +911,39 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -967,19 +951,19 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5" t="n">
         <v>20</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
@@ -987,59 +971,43 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1047,19 +1015,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1067,39 +1035,31 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5" t="n">
         <v>26</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1107,19 +1067,19 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <v>26</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1127,43 +1087,51 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1171,51 +1139,43 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1223,19 +1183,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1243,19 +1203,19 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1263,31 +1223,39 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1295,43 +1263,51 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1339,19 +1315,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1359,19 +1335,19 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>13</v>
@@ -1379,39 +1355,31 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1419,19 +1387,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1439,31 +1407,31 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1471,19 +1439,19 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1491,103 +1459,87 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1598,16 +1550,16 @@
         <v>75</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1615,67 +1567,83 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="B52" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E52" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>13</v>
@@ -1683,19 +1651,19 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1703,19 +1671,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1723,190 +1691,66 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E57" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F65">
+  <conditionalFormatting sqref="A5:F58">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1917,7 +1761,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A65">
+  <conditionalFormatting sqref="A5:A58">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 02.05.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 25 April 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 02 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -152,13 +152,22 @@
     <t xml:space="preserve">31 July 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Offender management statistics quarterly: January 2025 to March 2025 </t>
   </si>
   <si>
     <t xml:space="preserve">Proven reoffending statistics: July 2023 and September 2023</t>
   </si>
   <si>
+    <t xml:space="preserve">Offender Employment Outcomes, update to March 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community Performance Annual, update to March 2025</t>
   </si>
   <si>
     <t xml:space="preserve">HMPPS Annual Digest, April 2024 to March 2025</t>
@@ -1283,31 +1292,39 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1315,19 +1332,19 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>13</v>
@@ -1335,51 +1352,51 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1387,19 +1404,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1407,31 +1424,31 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1439,19 +1456,19 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>13</v>
@@ -1459,39 +1476,55 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E43" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
@@ -1501,7 +1534,7 @@
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F45" s="5"/>
     </row>
@@ -1509,101 +1542,93 @@
       <c r="A46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E49" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E50" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>13</v>
@@ -1611,59 +1636,43 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F52" s="5"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="E53" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F53" s="5"/>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>13</v>
@@ -1671,19 +1680,19 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>13</v>
@@ -1691,19 +1700,19 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>13</v>
@@ -1711,19 +1720,19 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>13</v>
@@ -1734,7 +1743,7 @@
         <v>95</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>97</v>
@@ -1743,14 +1752,74 @@
         <v>12</v>
       </c>
       <c r="E58" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F59" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F58">
+  <conditionalFormatting sqref="A5:F61">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1761,7 +1830,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A58">
+  <conditionalFormatting sqref="A5:A61">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 16.05.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 02 May 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 16 May 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,84 +41,45 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">05 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unpaid Work Management Information, update to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 May 2025</t>
+    <t xml:space="preserve">02 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil justice statistics: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
   </si>
   <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroners statistics 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM Prison and Probation Service workforce quarterly: March 2025.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage and landlord possession statistics: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First time entrants (FTE) into the Criminal Justice System and Offender Histories: year ending December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal justice statistics quarterly: December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knife and Offensive Weapon Sentencing Statistics:  October to December 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 May 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 June 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 June 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 June 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
   </si>
   <si>
@@ -128,13 +89,13 @@
     <t xml:space="preserve">30 Jun 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 July 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">07 Jul 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">14 Jul 2025</t>
@@ -756,7 +717,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="108.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="85.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="10.71" hidden="1" customWidth="1"/>
@@ -812,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -820,19 +781,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -840,39 +801,31 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
       <c r="E7" t="n">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -880,19 +833,19 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -900,19 +853,19 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -920,19 +873,19 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -940,83 +893,75 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E15" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -1024,19 +969,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -1044,31 +989,39 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1076,19 +1029,19 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1096,19 +1049,19 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>13</v>
@@ -1116,31 +1069,39 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1154,7 +1115,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -1162,29 +1123,37 @@
       <c r="A25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1192,19 +1161,19 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1212,39 +1181,31 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>13</v>
@@ -1252,19 +1213,19 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1272,39 +1233,31 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1312,19 +1265,19 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -1332,91 +1285,67 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1424,31 +1353,39 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1456,51 +1393,43 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1508,19 +1437,19 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>13</v>
@@ -1528,67 +1457,99 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E45" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E47" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E48" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1596,230 +1557,26 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F61">
+  <conditionalFormatting sqref="A5:F50">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1830,7 +1587,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A61">
+  <conditionalFormatting sqref="A5:A50">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 06.06.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 30 May 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">02 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civil justice statistics: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 June 2025</t>
+    <t xml:space="preserve">09 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
@@ -56,13 +56,7 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">09 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 June 2025</t>
+    <t xml:space="preserve">Identified offender needs, custody and community, 31st Oct 2024</t>
   </si>
   <si>
     <t xml:space="preserve">16 Jun 2025</t>
@@ -128,6 +122,9 @@
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Justice data lab statistics: July 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Community Performance Annual, update to March 2025</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
     <t xml:space="preserve">25 September 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Education and Accredited Programme Statistics 2024 to 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Legal aid statistics quarterly: April to June 2025</t>
   </si>
   <si>
@@ -212,12 +212,15 @@
     <t xml:space="preserve">27 Oct 2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Justice data lab statistics: October 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 October 2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Safety in custody: quarterly update to June 2025</t>
   </si>
   <si>
-    <t xml:space="preserve">30 October 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proven reoffending statistics: October to December 2023</t>
   </si>
   <si>
@@ -228,6 +231,12 @@
   </si>
   <si>
     <t xml:space="preserve">10 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison Population Projections: 2025 to 2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 November 2025</t>
   </si>
   <si>
     <t xml:space="preserve">17 Nov 2025</t>
@@ -773,7 +782,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -781,13 +790,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -801,7 +810,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
@@ -813,16 +822,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
         <v>26</v>
@@ -833,16 +842,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>26</v>
@@ -853,16 +862,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>26</v>
@@ -873,13 +882,13 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -893,7 +902,7 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -905,7 +914,7 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -917,7 +926,7 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -929,16 +938,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>31</v>
@@ -949,16 +958,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>31</v>
@@ -969,16 +978,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>31</v>
@@ -989,16 +998,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>31</v>
@@ -1009,16 +1018,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>31</v>
@@ -1029,16 +1038,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>31</v>
@@ -1049,16 +1058,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>31</v>
@@ -1069,16 +1078,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>31</v>
@@ -1089,16 +1098,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>31</v>
@@ -1109,51 +1118,51 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -1161,16 +1170,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>34</v>
@@ -1181,51 +1190,51 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E28" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1233,48 +1242,48 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E31" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F32" s="5"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>39</v>
@@ -1285,104 +1294,104 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>44</v>
@@ -1393,43 +1402,59 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="E42" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1437,39 +1462,31 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1477,19 +1494,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1497,19 +1514,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1517,19 +1534,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1537,19 +1554,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1560,23 +1577,83 @@
         <v>85</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E50" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F51" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F50">
+  <conditionalFormatting sqref="A5:F53">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1587,7 +1664,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A50">
+  <conditionalFormatting sqref="A5:A53">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 13.06.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 06 June 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 13 June 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,52 +41,37 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">09 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribunals statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 June 2025</t>
+    <t xml:space="preserve">23 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 June 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provisional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Jun 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified offender needs, custody and community, 31st Oct 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 June 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">provisional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">07 Jul 2025</t>
@@ -782,7 +767,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -802,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -810,15 +795,23 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" t="n">
-        <v>25</v>
-      </c>
-      <c r="F7"/>
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -834,7 +827,7 @@
         <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -842,112 +835,112 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5" t="n">
-        <v>26</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>31</v>
@@ -958,16 +951,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>31</v>
@@ -978,16 +971,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>31</v>
@@ -998,16 +991,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>31</v>
@@ -1018,16 +1011,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>31</v>
@@ -1038,16 +1031,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>31</v>
@@ -1058,16 +1051,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>31</v>
@@ -1078,39 +1071,31 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1118,19 +1103,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1138,35 +1123,35 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
@@ -1179,10 +1164,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>13</v>
@@ -1190,19 +1175,19 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>13</v>
@@ -1210,31 +1195,31 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1242,19 +1227,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1262,136 +1247,144 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E32" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E37" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E38" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E39" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>44</v>
@@ -1402,39 +1395,31 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1442,19 +1427,19 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
@@ -1462,31 +1447,39 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E44" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>13</v>
@@ -1494,19 +1487,19 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>13</v>
@@ -1514,19 +1507,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>13</v>
@@ -1534,19 +1527,19 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>13</v>
@@ -1554,19 +1547,19 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>13</v>
@@ -1574,86 +1567,26 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F53">
+  <conditionalFormatting sqref="A5:F50">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1664,7 +1597,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A53">
+  <conditionalFormatting sqref="A5:A50">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 04.07.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 20 June 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 04 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -41,13 +41,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">23 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal court statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 June 2025</t>
+    <t xml:space="preserve">28 Jul 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety in custody: quarterly update to March 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">provisional</t>
@@ -56,42 +56,6 @@
     <t xml:space="preserve">standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal aid statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family court statistics quarterly: January to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 Jun 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversity of the judiciary: 2025 statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 July 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 Jul 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 Jul 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Jul 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 Jul 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety in custody: quarterly update to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 July 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Offender Accommodation Outcomes, update to March 2025</t>
   </si>
   <si>
@@ -105,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">Safety in the children and young people secure estate: Update to March 2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justice data lab statistics: July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Community Performance Annual, update to March 2025</t>
@@ -767,7 +728,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -787,7 +748,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -807,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -815,19 +776,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -835,49 +796,73 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -891,13 +876,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -911,30 +896,22 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>25</v>
@@ -943,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>13</v>
@@ -951,19 +928,19 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -971,19 +948,19 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>13</v>
@@ -991,39 +968,31 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>13</v>
@@ -1031,19 +1000,19 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1051,51 +1020,51 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E22" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -1103,19 +1072,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5" t="n">
         <v>39</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>34</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -1123,103 +1092,87 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>13</v>
@@ -1227,19 +1180,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -1247,19 +1200,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -1267,67 +1220,91 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E33" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E35" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>13</v>
@@ -1335,19 +1312,19 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>13</v>
@@ -1355,19 +1332,19 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>13</v>
@@ -1375,19 +1352,19 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>13</v>
@@ -1395,31 +1372,39 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E41" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>13</v>
@@ -1430,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>72</v>
@@ -1439,154 +1424,14 @@
         <v>12</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:F50">
+  <conditionalFormatting sqref="A5:F43">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0)</formula>
     </cfRule>
@@ -1597,7 +1442,7 @@
       <formula>=AND($E5&lt;&gt;$E4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A50">
+  <conditionalFormatting sqref="A5:A43">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>=AND(LEN($E5)&gt;0,MOD(RIGHT($E5,2),2)=0,$E5=$E4)</formula>
     </cfRule>

</xml_diff>

<commit_message>
weekly forward look stats update 25.07.25
</commit_message>
<xml_diff>
--- a/Forward Look/Forward Look.xlsx
+++ b/Forward Look/Forward Look.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t xml:space="preserve">MoJ Statistics Forward Look</t>
   </si>
   <si>
-    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 17 July 2025</t>
+    <t xml:space="preserve">This list contains a week-by-week view of  MoJ Official and National Statistics that have been pre-announced on the gov.uk release calendar as at 25 July 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Click here to view on the gov.uk Research and Statistics calendar</t>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">Prison Performance Ratings: 2024 to 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Determinate Sentence (SDS40) release data</t>
   </si>
   <si>
     <t xml:space="preserve">04 Aug 2025</t>
@@ -896,51 +899,51 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>13</v>
@@ -948,13 +951,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -968,51 +971,51 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E18" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5" t="n">
         <v>36</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>13</v>
@@ -1020,45 +1023,45 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>12</v>
@@ -1072,13 +1075,13 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>12</v>
@@ -1092,15 +1095,23 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E25" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
@@ -1110,7 +1121,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -1122,7 +1133,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -1134,7 +1145,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1142,31 +1153,23 @@
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>12</v>
@@ -1180,13 +1183,13 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>12</v>
@@ -1200,13 +1203,13 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>12</v>
@@ -1220,13 +1223,13 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>12</v>
@@ -1240,51 +1243,51 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E34" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="5" t="